<commit_message>
update language - include Shona
update French language to Shona
</commit_message>
<xml_diff>
--- a/ebs_with_tracing/forms/app/declaration.xlsx
+++ b/ebs_with_tracing/forms/app/declaration.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10308"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/senseibara/Documents/MEDIC/config-cht-demo/forms/app/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Github\config-covid\forms\app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5EC8FBE-90AF-624C-AD48-63058158B155}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -18,10 +17,10 @@
     <sheet name="settings" sheetId="3" r:id="rId3"/>
     <sheet name="choices-backup" sheetId="4" state="hidden" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
+      <x14:workbookPr defaultImageDpi="330"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="246">
   <si>
     <t>form_title</t>
   </si>
@@ -734,12 +733,6 @@
     <t>Remarques</t>
   </si>
   <si>
-    <t>Oui</t>
-  </si>
-  <si>
-    <t>Non</t>
-  </si>
-  <si>
     <t>Informations du contact</t>
   </si>
   <si>
@@ -783,16 +776,25 @@
   </si>
   <si>
     <t>string</t>
+  </si>
+  <si>
+    <t>label::sh</t>
+  </si>
+  <si>
+    <t>Hongu</t>
+  </si>
+  <si>
+    <t>Kwete</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd\-mm\-yyyy\ hh\-mm\-ss"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1326,38 +1328,38 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:AB82"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C25" sqref="C25"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="21.33203125" customWidth="1"/>
-    <col min="2" max="2" width="33.33203125" customWidth="1"/>
-    <col min="3" max="4" width="43.33203125" customWidth="1"/>
-    <col min="5" max="5" width="14.5" customWidth="1"/>
-    <col min="6" max="6" width="53.83203125" customWidth="1"/>
-    <col min="7" max="7" width="32.33203125" customWidth="1"/>
-    <col min="8" max="9" width="17.5" customWidth="1"/>
-    <col min="10" max="10" width="10.83203125" customWidth="1"/>
-    <col min="11" max="11" width="22.6640625" customWidth="1"/>
-    <col min="12" max="12" width="73.83203125" customWidth="1"/>
-    <col min="13" max="13" width="14.5" customWidth="1"/>
+    <col min="1" max="1" width="21.28515625" customWidth="1"/>
+    <col min="2" max="2" width="33.28515625" customWidth="1"/>
+    <col min="3" max="4" width="43.28515625" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" customWidth="1"/>
+    <col min="6" max="6" width="53.85546875" customWidth="1"/>
+    <col min="7" max="7" width="32.28515625" customWidth="1"/>
+    <col min="8" max="9" width="17.42578125" customWidth="1"/>
+    <col min="10" max="10" width="10.85546875" customWidth="1"/>
+    <col min="11" max="11" width="22.7109375" customWidth="1"/>
+    <col min="12" max="12" width="73.85546875" customWidth="1"/>
+    <col min="13" max="13" width="14.42578125" customWidth="1"/>
     <col min="14" max="14" width="30" customWidth="1"/>
-    <col min="15" max="15" width="14.5" customWidth="1"/>
-    <col min="16" max="28" width="29.83203125" customWidth="1"/>
+    <col min="15" max="15" width="14.42578125" customWidth="1"/>
+    <col min="16" max="28" width="29.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:28" ht="15.75" customHeight="1">
       <c r="A1" s="3" t="s">
         <v>7</v>
       </c>
@@ -1368,7 +1370,7 @@
         <v>10</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>69</v>
+        <v>243</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>11</v>
@@ -1427,7 +1429,7 @@
       <c r="AA1" s="7"/>
       <c r="AB1" s="7"/>
     </row>
-    <row r="2" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:28" ht="15.75" customHeight="1">
       <c r="A2" s="12" t="s">
         <v>29</v>
       </c>
@@ -1467,7 +1469,7 @@
       <c r="AA2" s="19"/>
       <c r="AB2" s="19"/>
     </row>
-    <row r="3" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:28" ht="15.75" customHeight="1">
       <c r="A3" s="12" t="s">
         <v>41</v>
       </c>
@@ -1505,7 +1507,7 @@
       <c r="AA3" s="19"/>
       <c r="AB3" s="19"/>
     </row>
-    <row r="4" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:28" ht="15.75" customHeight="1">
       <c r="A4" s="12" t="s">
         <v>41</v>
       </c>
@@ -1541,7 +1543,7 @@
       <c r="AA4" s="19"/>
       <c r="AB4" s="19"/>
     </row>
-    <row r="5" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:28" ht="15.75" customHeight="1">
       <c r="A5" s="12" t="s">
         <v>29</v>
       </c>
@@ -1577,7 +1579,7 @@
       <c r="AA5" s="19"/>
       <c r="AB5" s="19"/>
     </row>
-    <row r="6" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:28" ht="15.75" customHeight="1">
       <c r="A6" s="12" t="s">
         <v>48</v>
       </c>
@@ -1615,7 +1617,7 @@
       <c r="AA6" s="19"/>
       <c r="AB6" s="19"/>
     </row>
-    <row r="7" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:28" ht="15.75" customHeight="1">
       <c r="A7" s="12" t="s">
         <v>41</v>
       </c>
@@ -1651,7 +1653,7 @@
       <c r="AA7" s="19"/>
       <c r="AB7" s="19"/>
     </row>
-    <row r="8" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:28" ht="15.75" customHeight="1">
       <c r="A8" s="12" t="s">
         <v>41</v>
       </c>
@@ -1687,7 +1689,7 @@
       <c r="AA8" s="19"/>
       <c r="AB8" s="19"/>
     </row>
-    <row r="9" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:28" ht="15.75" customHeight="1">
       <c r="A9" s="12" t="s">
         <v>55</v>
       </c>
@@ -1721,7 +1723,7 @@
       <c r="AA9" s="19"/>
       <c r="AB9" s="19"/>
     </row>
-    <row r="10" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:28" ht="15.75" customHeight="1">
       <c r="A10" s="12" t="s">
         <v>55</v>
       </c>
@@ -1757,7 +1759,7 @@
       <c r="AA10" s="19"/>
       <c r="AB10" s="19"/>
     </row>
-    <row r="11" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:28" ht="15.75" customHeight="1">
       <c r="A11" s="23"/>
       <c r="B11" s="23"/>
       <c r="C11" s="23"/>
@@ -1787,7 +1789,7 @@
       <c r="AA11" s="25"/>
       <c r="AB11" s="25"/>
     </row>
-    <row r="12" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:28" ht="15.75" customHeight="1">
       <c r="A12" s="26" t="s">
         <v>56</v>
       </c>
@@ -1825,7 +1827,7 @@
       <c r="AA12" s="29"/>
       <c r="AB12" s="29"/>
     </row>
-    <row r="13" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:28" ht="15.75" customHeight="1">
       <c r="A13" s="26" t="s">
         <v>56</v>
       </c>
@@ -1863,7 +1865,7 @@
       <c r="AA13" s="29"/>
       <c r="AB13" s="29"/>
     </row>
-    <row r="14" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:28" ht="15.75" customHeight="1">
       <c r="A14" s="26" t="s">
         <v>56</v>
       </c>
@@ -1901,7 +1903,7 @@
       <c r="AA14" s="29"/>
       <c r="AB14" s="29"/>
     </row>
-    <row r="15" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:28" ht="15.75" customHeight="1">
       <c r="A15" s="32" t="s">
         <v>56</v>
       </c>
@@ -1939,7 +1941,7 @@
       <c r="AA15" s="29"/>
       <c r="AB15" s="29"/>
     </row>
-    <row r="16" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:28" ht="15.75" customHeight="1">
       <c r="A16" s="23"/>
       <c r="B16" s="24"/>
       <c r="C16" s="24"/>
@@ -1969,7 +1971,7 @@
       <c r="AA16" s="37"/>
       <c r="AB16" s="37"/>
     </row>
-    <row r="17" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:28" ht="15.75" customHeight="1">
       <c r="A17" s="39" t="s">
         <v>29</v>
       </c>
@@ -2009,7 +2011,7 @@
       <c r="AA17" s="41"/>
       <c r="AB17" s="41"/>
     </row>
-    <row r="18" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:28" ht="15.75" customHeight="1">
       <c r="A18" s="46" t="s">
         <v>117</v>
       </c>
@@ -2047,7 +2049,7 @@
       <c r="AA18" s="41"/>
       <c r="AB18" s="41"/>
     </row>
-    <row r="19" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:28" ht="15.75" customHeight="1">
       <c r="A19" s="39" t="s">
         <v>120</v>
       </c>
@@ -2058,7 +2060,7 @@
         <v>122</v>
       </c>
       <c r="D19" s="52" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="E19" s="41"/>
       <c r="F19" s="41"/>
@@ -2085,9 +2087,9 @@
       <c r="AA19" s="41"/>
       <c r="AB19" s="41"/>
     </row>
-    <row r="20" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:28" ht="15.75" customHeight="1">
       <c r="A20" s="46" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B20" s="39" t="s">
         <v>130</v>
@@ -2123,9 +2125,9 @@
       <c r="AA20" s="41"/>
       <c r="AB20" s="41"/>
     </row>
-    <row r="21" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:28" ht="15.75" customHeight="1">
       <c r="A21" s="46" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B21" s="39" t="s">
         <v>134</v>
@@ -2134,7 +2136,7 @@
         <v>135</v>
       </c>
       <c r="D21" s="47" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="E21" s="41"/>
       <c r="F21" s="41"/>
@@ -2161,7 +2163,7 @@
       <c r="AA21" s="41"/>
       <c r="AB21" s="41"/>
     </row>
-    <row r="22" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:28" ht="15.75" customHeight="1">
       <c r="A22" s="39" t="s">
         <v>136</v>
       </c>
@@ -2193,7 +2195,7 @@
       <c r="AA22" s="41"/>
       <c r="AB22" s="41"/>
     </row>
-    <row r="23" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:28" ht="15.75" customHeight="1">
       <c r="A23" s="39" t="s">
         <v>55</v>
       </c>
@@ -2225,7 +2227,7 @@
       <c r="AA23" s="41"/>
       <c r="AB23" s="41"/>
     </row>
-    <row r="24" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:28" ht="15.75" customHeight="1">
       <c r="A24" s="49"/>
       <c r="B24" s="49"/>
       <c r="C24" s="50"/>
@@ -2255,7 +2257,7 @@
       <c r="AA24" s="50"/>
       <c r="AB24" s="50"/>
     </row>
-    <row r="25" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:28" ht="15.75" customHeight="1">
       <c r="A25" s="39" t="s">
         <v>29</v>
       </c>
@@ -2266,7 +2268,7 @@
         <v>164</v>
       </c>
       <c r="D25" s="47" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="E25" s="41"/>
       <c r="F25" s="42"/>
@@ -2293,7 +2295,7 @@
       <c r="AA25" s="41"/>
       <c r="AB25" s="41"/>
     </row>
-    <row r="26" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:28" ht="15.75" customHeight="1">
       <c r="A26" s="39" t="s">
         <v>179</v>
       </c>
@@ -2331,7 +2333,7 @@
       <c r="AA26" s="41"/>
       <c r="AB26" s="41"/>
     </row>
-    <row r="27" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:28" ht="15.75" customHeight="1">
       <c r="A27" s="39" t="s">
         <v>179</v>
       </c>
@@ -2342,7 +2344,7 @@
         <v>187</v>
       </c>
       <c r="D27" s="52" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E27" s="45"/>
       <c r="F27" s="41"/>
@@ -2369,7 +2371,7 @@
       <c r="AA27" s="41"/>
       <c r="AB27" s="41"/>
     </row>
-    <row r="28" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:28" ht="15.75" customHeight="1">
       <c r="A28" s="39" t="s">
         <v>179</v>
       </c>
@@ -2380,7 +2382,7 @@
         <v>189</v>
       </c>
       <c r="D28" s="52" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="E28" s="45"/>
       <c r="F28" s="41"/>
@@ -2407,7 +2409,7 @@
       <c r="AA28" s="41"/>
       <c r="AB28" s="41"/>
     </row>
-    <row r="29" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:28" ht="15.75" customHeight="1">
       <c r="A29" s="39" t="s">
         <v>179</v>
       </c>
@@ -2418,7 +2420,7 @@
         <v>191</v>
       </c>
       <c r="D29" s="52" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="E29" s="41"/>
       <c r="F29" s="41"/>
@@ -2445,7 +2447,7 @@
       <c r="AA29" s="41"/>
       <c r="AB29" s="41"/>
     </row>
-    <row r="30" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:28" ht="15.75" customHeight="1">
       <c r="A30" s="46" t="s">
         <v>56</v>
       </c>
@@ -2481,7 +2483,7 @@
       <c r="AA30" s="41"/>
       <c r="AB30" s="41"/>
     </row>
-    <row r="31" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:28" ht="15.75" customHeight="1">
       <c r="A31" s="39" t="s">
         <v>55</v>
       </c>
@@ -2513,7 +2515,7 @@
       <c r="AA31" s="41"/>
       <c r="AB31" s="41"/>
     </row>
-    <row r="32" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:28" ht="15.75" customHeight="1">
       <c r="A32" s="49"/>
       <c r="B32" s="50"/>
       <c r="C32" s="49"/>
@@ -2543,7 +2545,7 @@
       <c r="AA32" s="50"/>
       <c r="AB32" s="50"/>
     </row>
-    <row r="33" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:28" ht="15.75" customHeight="1">
       <c r="A33" s="39" t="s">
         <v>29</v>
       </c>
@@ -2581,7 +2583,7 @@
       <c r="AA33" s="41"/>
       <c r="AB33" s="41"/>
     </row>
-    <row r="34" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:28" ht="15.75" customHeight="1">
       <c r="A34" s="39" t="s">
         <v>179</v>
       </c>
@@ -2592,7 +2594,7 @@
         <v>199</v>
       </c>
       <c r="D34" s="52" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="E34" s="45"/>
       <c r="F34" s="42"/>
@@ -2619,7 +2621,7 @@
       <c r="AA34" s="41"/>
       <c r="AB34" s="41"/>
     </row>
-    <row r="35" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:28" ht="15.75" customHeight="1">
       <c r="A35" s="39" t="s">
         <v>179</v>
       </c>
@@ -2630,7 +2632,7 @@
         <v>201</v>
       </c>
       <c r="D35" s="52" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="E35" s="45"/>
       <c r="F35" s="42"/>
@@ -2657,7 +2659,7 @@
       <c r="AA35" s="41"/>
       <c r="AB35" s="41"/>
     </row>
-    <row r="36" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:28" ht="15.75" customHeight="1">
       <c r="A36" s="39" t="s">
         <v>179</v>
       </c>
@@ -2668,7 +2670,7 @@
         <v>203</v>
       </c>
       <c r="D36" s="52" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="E36" s="45"/>
       <c r="F36" s="44"/>
@@ -2695,7 +2697,7 @@
       <c r="AA36" s="41"/>
       <c r="AB36" s="41"/>
     </row>
-    <row r="37" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:28" ht="15.75" customHeight="1">
       <c r="A37" s="39" t="s">
         <v>179</v>
       </c>
@@ -2706,7 +2708,7 @@
         <v>205</v>
       </c>
       <c r="D37" s="47" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="E37" s="41"/>
       <c r="F37" s="42"/>
@@ -2733,7 +2735,7 @@
       <c r="AA37" s="41"/>
       <c r="AB37" s="41"/>
     </row>
-    <row r="38" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:28" ht="15.75" customHeight="1">
       <c r="A38" s="39" t="s">
         <v>179</v>
       </c>
@@ -2744,7 +2746,7 @@
         <v>207</v>
       </c>
       <c r="D38" s="47" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="E38" s="41"/>
       <c r="F38" s="42"/>
@@ -2771,7 +2773,7 @@
       <c r="AA38" s="41"/>
       <c r="AB38" s="41"/>
     </row>
-    <row r="39" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:28" ht="15.75" customHeight="1">
       <c r="A39" s="39" t="s">
         <v>179</v>
       </c>
@@ -2782,7 +2784,7 @@
         <v>209</v>
       </c>
       <c r="D39" s="47" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="E39" s="41"/>
       <c r="F39" s="42"/>
@@ -2809,7 +2811,7 @@
       <c r="AA39" s="41"/>
       <c r="AB39" s="41"/>
     </row>
-    <row r="40" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:28" ht="15.75" customHeight="1">
       <c r="A40" s="39" t="s">
         <v>179</v>
       </c>
@@ -2820,7 +2822,7 @@
         <v>211</v>
       </c>
       <c r="D40" s="47" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="E40" s="41"/>
       <c r="F40" s="42"/>
@@ -2847,7 +2849,7 @@
       <c r="AA40" s="41"/>
       <c r="AB40" s="41"/>
     </row>
-    <row r="41" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:28" ht="15.75" customHeight="1">
       <c r="A41" s="39" t="s">
         <v>179</v>
       </c>
@@ -2858,7 +2860,7 @@
         <v>213</v>
       </c>
       <c r="D41" s="47" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="E41" s="41"/>
       <c r="F41" s="42"/>
@@ -2885,7 +2887,7 @@
       <c r="AA41" s="41"/>
       <c r="AB41" s="41"/>
     </row>
-    <row r="42" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:28" ht="15.75" customHeight="1">
       <c r="A42" s="39" t="s">
         <v>179</v>
       </c>
@@ -2923,7 +2925,7 @@
       <c r="AA42" s="41"/>
       <c r="AB42" s="41"/>
     </row>
-    <row r="43" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:28" ht="15.75" customHeight="1">
       <c r="A43" s="46" t="s">
         <v>117</v>
       </c>
@@ -2965,7 +2967,7 @@
       <c r="AA43" s="41"/>
       <c r="AB43" s="41"/>
     </row>
-    <row r="44" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:28" ht="15.75" customHeight="1">
       <c r="A44" s="46" t="s">
         <v>56</v>
       </c>
@@ -3001,7 +3003,7 @@
       <c r="AA44" s="41"/>
       <c r="AB44" s="41"/>
     </row>
-    <row r="45" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:28" ht="15.75" customHeight="1">
       <c r="A45" s="39" t="s">
         <v>55</v>
       </c>
@@ -3033,7 +3035,7 @@
       <c r="AA45" s="41"/>
       <c r="AB45" s="41"/>
     </row>
-    <row r="46" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:28" ht="15.75" customHeight="1">
       <c r="A46" s="53"/>
       <c r="B46" s="53"/>
       <c r="C46" s="53"/>
@@ -3041,7 +3043,7 @@
       <c r="F46" s="53"/>
       <c r="G46" s="53"/>
     </row>
-    <row r="47" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:28" ht="15.75" customHeight="1">
       <c r="A47" s="53"/>
       <c r="B47" s="53"/>
       <c r="C47" s="53"/>
@@ -3049,7 +3051,7 @@
       <c r="F47" s="53"/>
       <c r="G47" s="53"/>
     </row>
-    <row r="48" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:28" ht="15.75" customHeight="1">
       <c r="A48" s="53"/>
       <c r="B48" s="53"/>
       <c r="C48" s="53"/>
@@ -3057,7 +3059,7 @@
       <c r="F48" s="53"/>
       <c r="G48" s="53"/>
     </row>
-    <row r="49" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:9" ht="15.75" customHeight="1">
       <c r="A49" s="53"/>
       <c r="B49" s="53"/>
       <c r="C49" s="53"/>
@@ -3065,7 +3067,7 @@
       <c r="F49" s="53"/>
       <c r="G49" s="53"/>
     </row>
-    <row r="50" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:9" ht="15.75" customHeight="1">
       <c r="A50" s="53"/>
       <c r="B50" s="53"/>
       <c r="C50" s="53"/>
@@ -3073,7 +3075,7 @@
       <c r="F50" s="53"/>
       <c r="G50" s="53"/>
     </row>
-    <row r="51" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:9" ht="15.75" customHeight="1">
       <c r="A51" s="53"/>
       <c r="B51" s="53"/>
       <c r="C51" s="53"/>
@@ -3083,7 +3085,7 @@
       <c r="H51" s="53"/>
       <c r="I51" s="53"/>
     </row>
-    <row r="52" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:9" ht="15.75" customHeight="1">
       <c r="A52" s="53"/>
       <c r="B52" s="53"/>
       <c r="C52" s="53"/>
@@ -3091,7 +3093,7 @@
       <c r="F52" s="53"/>
       <c r="G52" s="53"/>
     </row>
-    <row r="53" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:9" ht="15.75" customHeight="1">
       <c r="A53" s="53"/>
       <c r="B53" s="53"/>
       <c r="C53" s="53"/>
@@ -3099,7 +3101,7 @@
       <c r="F53" s="53"/>
       <c r="G53" s="53"/>
     </row>
-    <row r="54" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:9" ht="15.75" customHeight="1">
       <c r="A54" s="53"/>
       <c r="B54" s="53"/>
       <c r="C54" s="53"/>
@@ -3107,7 +3109,7 @@
       <c r="F54" s="53"/>
       <c r="G54" s="53"/>
     </row>
-    <row r="55" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:9" ht="15.75" customHeight="1">
       <c r="A55" s="53"/>
       <c r="B55" s="53"/>
       <c r="C55" s="53"/>
@@ -3115,7 +3117,7 @@
       <c r="F55" s="53"/>
       <c r="G55" s="53"/>
     </row>
-    <row r="56" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:9" ht="15.75" customHeight="1">
       <c r="A56" s="53"/>
       <c r="B56" s="53"/>
       <c r="C56" s="53"/>
@@ -3123,7 +3125,7 @@
       <c r="F56" s="53"/>
       <c r="G56" s="53"/>
     </row>
-    <row r="57" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:9" ht="15.75" customHeight="1">
       <c r="A57" s="53"/>
       <c r="B57" s="53"/>
       <c r="C57" s="53"/>
@@ -3131,7 +3133,7 @@
       <c r="F57" s="53"/>
       <c r="G57" s="53"/>
     </row>
-    <row r="58" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:9" ht="15.75" customHeight="1">
       <c r="A58" s="53"/>
       <c r="B58" s="53"/>
       <c r="C58" s="53"/>
@@ -3139,7 +3141,7 @@
       <c r="F58" s="53"/>
       <c r="G58" s="53"/>
     </row>
-    <row r="59" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:9" ht="15.75" customHeight="1">
       <c r="A59" s="53"/>
       <c r="B59" s="53"/>
       <c r="C59" s="53"/>
@@ -3147,7 +3149,7 @@
       <c r="F59" s="53"/>
       <c r="G59" s="53"/>
     </row>
-    <row r="60" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:9" ht="15.75" customHeight="1">
       <c r="A60" s="53"/>
       <c r="B60" s="53"/>
       <c r="C60" s="53"/>
@@ -3155,7 +3157,7 @@
       <c r="F60" s="53"/>
       <c r="G60" s="53"/>
     </row>
-    <row r="61" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:9" ht="15.75" customHeight="1">
       <c r="A61" s="53"/>
       <c r="B61" s="53"/>
       <c r="C61" s="53"/>
@@ -3165,7 +3167,7 @@
       <c r="H61" s="53"/>
       <c r="I61" s="53"/>
     </row>
-    <row r="62" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:9" ht="15.75" customHeight="1">
       <c r="A62" s="53"/>
       <c r="B62" s="53"/>
       <c r="C62" s="53"/>
@@ -3175,7 +3177,7 @@
       <c r="H62" s="53"/>
       <c r="I62" s="53"/>
     </row>
-    <row r="63" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:9" ht="15.75" customHeight="1">
       <c r="A63" s="53"/>
       <c r="B63" s="53"/>
       <c r="C63" s="53"/>
@@ -3185,7 +3187,7 @@
       <c r="H63" s="53"/>
       <c r="I63" s="53"/>
     </row>
-    <row r="64" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:9" ht="15.75" customHeight="1">
       <c r="A64" s="53"/>
       <c r="B64" s="53"/>
       <c r="C64" s="53"/>
@@ -3195,7 +3197,7 @@
       <c r="H64" s="53"/>
       <c r="I64" s="53"/>
     </row>
-    <row r="65" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:9" ht="15.75" customHeight="1">
       <c r="A65" s="53"/>
       <c r="B65" s="53"/>
       <c r="C65" s="53"/>
@@ -3205,7 +3207,7 @@
       <c r="H65" s="53"/>
       <c r="I65" s="53"/>
     </row>
-    <row r="66" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:9" ht="15.75" customHeight="1">
       <c r="A66" s="53"/>
       <c r="B66" s="53"/>
       <c r="C66" s="53"/>
@@ -3215,7 +3217,7 @@
       <c r="H66" s="53"/>
       <c r="I66" s="53"/>
     </row>
-    <row r="67" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="67" spans="1:9" ht="15.75" customHeight="1">
       <c r="A67" s="53"/>
       <c r="B67" s="53"/>
       <c r="C67" s="53"/>
@@ -3225,7 +3227,7 @@
       <c r="H67" s="53"/>
       <c r="I67" s="53"/>
     </row>
-    <row r="68" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="68" spans="1:9" ht="15.75" customHeight="1">
       <c r="A68" s="53"/>
       <c r="B68" s="53"/>
       <c r="C68" s="53"/>
@@ -3235,7 +3237,7 @@
       <c r="H68" s="53"/>
       <c r="I68" s="53"/>
     </row>
-    <row r="69" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="69" spans="1:9" ht="15.75" customHeight="1">
       <c r="A69" s="53"/>
       <c r="B69" s="53"/>
       <c r="C69" s="53"/>
@@ -3245,7 +3247,7 @@
       <c r="H69" s="53"/>
       <c r="I69" s="53"/>
     </row>
-    <row r="70" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:9" ht="15.75" customHeight="1">
       <c r="A70" s="53"/>
       <c r="B70" s="53"/>
       <c r="C70" s="53"/>
@@ -3255,7 +3257,7 @@
       <c r="H70" s="53"/>
       <c r="I70" s="53"/>
     </row>
-    <row r="71" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="71" spans="1:9" ht="15.75" customHeight="1">
       <c r="A71" s="53"/>
       <c r="B71" s="53"/>
       <c r="C71" s="53"/>
@@ -3265,7 +3267,7 @@
       <c r="H71" s="53"/>
       <c r="I71" s="53"/>
     </row>
-    <row r="72" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="72" spans="1:9" ht="15.75" customHeight="1">
       <c r="A72" s="53"/>
       <c r="B72" s="53"/>
       <c r="C72" s="53"/>
@@ -3275,7 +3277,7 @@
       <c r="H72" s="53"/>
       <c r="I72" s="53"/>
     </row>
-    <row r="73" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="73" spans="1:9" ht="15.75" customHeight="1">
       <c r="A73" s="53"/>
       <c r="B73" s="53"/>
       <c r="C73" s="53"/>
@@ -3285,7 +3287,7 @@
       <c r="H73" s="53"/>
       <c r="I73" s="53"/>
     </row>
-    <row r="74" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="74" spans="1:9" ht="15.75" customHeight="1">
       <c r="A74" s="53"/>
       <c r="B74" s="53"/>
       <c r="C74" s="53"/>
@@ -3295,7 +3297,7 @@
       <c r="H74" s="53"/>
       <c r="I74" s="53"/>
     </row>
-    <row r="75" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="75" spans="1:9" ht="15.75" customHeight="1">
       <c r="A75" s="53"/>
       <c r="B75" s="53"/>
       <c r="C75" s="53"/>
@@ -3305,7 +3307,7 @@
       <c r="H75" s="53"/>
       <c r="I75" s="53"/>
     </row>
-    <row r="76" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="76" spans="1:9" ht="15.75" customHeight="1">
       <c r="A76" s="53"/>
       <c r="B76" s="53"/>
       <c r="C76" s="53"/>
@@ -3315,7 +3317,7 @@
       <c r="H76" s="53"/>
       <c r="I76" s="53"/>
     </row>
-    <row r="77" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="77" spans="1:9" ht="15.75" customHeight="1">
       <c r="A77" s="53"/>
       <c r="B77" s="53"/>
       <c r="C77" s="53"/>
@@ -3325,7 +3327,7 @@
       <c r="H77" s="53"/>
       <c r="I77" s="53"/>
     </row>
-    <row r="78" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="78" spans="1:9" ht="15.75" customHeight="1">
       <c r="A78" s="53"/>
       <c r="B78" s="53"/>
       <c r="C78" s="53"/>
@@ -3335,7 +3337,7 @@
       <c r="H78" s="53"/>
       <c r="I78" s="53"/>
     </row>
-    <row r="79" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="79" spans="1:9" ht="15.75" customHeight="1">
       <c r="A79" s="53"/>
       <c r="B79" s="53"/>
       <c r="C79" s="53"/>
@@ -3345,7 +3347,7 @@
       <c r="H79" s="53"/>
       <c r="I79" s="53"/>
     </row>
-    <row r="80" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="80" spans="1:9" ht="15.75" customHeight="1">
       <c r="A80" s="53"/>
       <c r="B80" s="53"/>
       <c r="C80" s="53"/>
@@ -3355,7 +3357,7 @@
       <c r="H80" s="53"/>
       <c r="I80" s="53"/>
     </row>
-    <row r="81" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="81" spans="1:9" ht="15.75" customHeight="1">
       <c r="A81" s="53"/>
       <c r="B81" s="53"/>
       <c r="C81" s="53"/>
@@ -3365,7 +3367,7 @@
       <c r="H81" s="53"/>
       <c r="I81" s="53"/>
     </row>
-    <row r="82" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="82" spans="1:9" ht="15.75" customHeight="1">
       <c r="A82" s="53"/>
       <c r="B82" s="53"/>
       <c r="C82" s="53"/>
@@ -3377,7 +3379,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" sqref="E2:E82" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" sqref="E2:E82">
       <formula1>"yes,no"</formula1>
     </dataValidation>
   </dataValidations>
@@ -3386,24 +3388,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:P67"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
+      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="28.33203125" customWidth="1"/>
-    <col min="2" max="16" width="45.83203125" customWidth="1"/>
+    <col min="1" max="1" width="28.28515625" customWidth="1"/>
+    <col min="2" max="16" width="45.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>27</v>
       </c>
@@ -3414,7 +3416,7 @@
         <v>10</v>
       </c>
       <c r="D1" s="54" t="s">
-        <v>69</v>
+        <v>243</v>
       </c>
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
@@ -3429,7 +3431,7 @@
       <c r="O1" s="10"/>
       <c r="P1" s="10"/>
     </row>
-    <row r="2" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" ht="15.75" customHeight="1">
       <c r="A2" s="15" t="s">
         <v>30</v>
       </c>
@@ -3440,7 +3442,7 @@
         <v>36</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>228</v>
+        <v>244</v>
       </c>
       <c r="E2" s="16"/>
       <c r="F2" s="16"/>
@@ -3455,7 +3457,7 @@
       <c r="O2" s="16"/>
       <c r="P2" s="16"/>
     </row>
-    <row r="3" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" ht="15.75" customHeight="1">
       <c r="A3" s="15" t="s">
         <v>30</v>
       </c>
@@ -3466,7 +3468,7 @@
         <v>38</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>229</v>
+        <v>245</v>
       </c>
       <c r="E3" s="16"/>
       <c r="F3" s="16"/>
@@ -3481,7 +3483,7 @@
       <c r="O3" s="16"/>
       <c r="P3" s="16"/>
     </row>
-    <row r="4" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:16" ht="15.75" customHeight="1">
       <c r="A4" s="10"/>
       <c r="B4" s="10"/>
       <c r="C4" s="18"/>
@@ -3499,193 +3501,193 @@
       <c r="O4" s="16"/>
       <c r="P4" s="16"/>
     </row>
-    <row r="5" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:16" ht="15.75" customHeight="1">
       <c r="C5" s="20"/>
     </row>
-    <row r="6" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:16" ht="15.75" customHeight="1">
       <c r="C6" s="20"/>
     </row>
-    <row r="7" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:16" ht="15.75" customHeight="1">
       <c r="C7" s="16"/>
     </row>
-    <row r="8" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:16" ht="15.75" customHeight="1">
       <c r="C8" s="16"/>
     </row>
-    <row r="9" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:16" ht="15.75" customHeight="1">
       <c r="C9" s="16"/>
     </row>
-    <row r="10" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:16" ht="15.75" customHeight="1">
       <c r="C10" s="16"/>
     </row>
-    <row r="11" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:16" ht="15.75" customHeight="1">
       <c r="C11" s="16"/>
     </row>
-    <row r="12" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:16" ht="15.75" customHeight="1">
       <c r="C12" s="16"/>
     </row>
-    <row r="13" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:16" ht="15.75" customHeight="1">
       <c r="C13" s="16"/>
     </row>
-    <row r="14" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:16" ht="15.75" customHeight="1">
       <c r="C14" s="16"/>
     </row>
-    <row r="15" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:16" ht="15.75" customHeight="1">
       <c r="C15" s="16"/>
     </row>
-    <row r="16" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:16" ht="15.75" customHeight="1">
       <c r="C16" s="16"/>
     </row>
-    <row r="17" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="3:3" ht="15.75" customHeight="1">
       <c r="C17" s="16"/>
     </row>
-    <row r="18" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="3:3" ht="15.75" customHeight="1">
       <c r="C18" s="16"/>
     </row>
-    <row r="19" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="3:3" ht="15.75" customHeight="1">
       <c r="C19" s="16"/>
     </row>
-    <row r="20" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="3:3" ht="15.75" customHeight="1">
       <c r="C20" s="16"/>
     </row>
-    <row r="21" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="3:3" ht="15.75" customHeight="1">
       <c r="C21" s="16"/>
     </row>
-    <row r="22" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="3:3" ht="15.75" customHeight="1">
       <c r="C22" s="16"/>
     </row>
-    <row r="23" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="3:3" ht="15.75" customHeight="1">
       <c r="C23" s="16"/>
     </row>
-    <row r="24" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="3:3" ht="15.75" customHeight="1">
       <c r="C24" s="16"/>
     </row>
-    <row r="25" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="3:3" ht="15.75" customHeight="1">
       <c r="C25" s="16"/>
     </row>
-    <row r="26" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="3:3" ht="15.75" customHeight="1">
       <c r="C26" s="16"/>
     </row>
-    <row r="27" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="3:3" ht="15.75" customHeight="1">
       <c r="C27" s="16"/>
     </row>
-    <row r="28" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="3:3" ht="15.75" customHeight="1">
       <c r="C28" s="16"/>
     </row>
-    <row r="29" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="3:3" ht="15.75" customHeight="1">
       <c r="C29" s="16"/>
     </row>
-    <row r="30" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="3:3" ht="15.75" customHeight="1">
       <c r="C30" s="16"/>
     </row>
-    <row r="31" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="3:3" ht="15.75" customHeight="1">
       <c r="C31" s="16"/>
     </row>
-    <row r="32" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="32" spans="3:3" ht="15.75" customHeight="1">
       <c r="C32" s="16"/>
     </row>
-    <row r="33" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="33" spans="3:3" ht="15.75" customHeight="1">
       <c r="C33" s="16"/>
     </row>
-    <row r="34" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="34" spans="3:3" ht="15.75" customHeight="1">
       <c r="C34" s="16"/>
     </row>
-    <row r="35" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="35" spans="3:3" ht="15.75" customHeight="1">
       <c r="C35" s="16"/>
     </row>
-    <row r="36" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="36" spans="3:3" ht="15.75" customHeight="1">
       <c r="C36" s="16"/>
     </row>
-    <row r="37" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="37" spans="3:3" ht="15.75" customHeight="1">
       <c r="C37" s="16"/>
     </row>
-    <row r="38" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="38" spans="3:3" ht="15.75" customHeight="1">
       <c r="C38" s="16"/>
     </row>
-    <row r="39" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="39" spans="3:3" ht="15.75" customHeight="1">
       <c r="C39" s="16"/>
     </row>
-    <row r="40" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="40" spans="3:3" ht="15.75" customHeight="1">
       <c r="C40" s="16"/>
     </row>
-    <row r="41" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="41" spans="3:3" ht="15.75" customHeight="1">
       <c r="C41" s="16"/>
     </row>
-    <row r="42" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="42" spans="3:3" ht="15.75" customHeight="1">
       <c r="C42" s="16"/>
     </row>
-    <row r="43" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="43" spans="3:3" ht="15.75" customHeight="1">
       <c r="C43" s="16"/>
     </row>
-    <row r="44" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="44" spans="3:3" ht="15.75" customHeight="1">
       <c r="C44" s="16"/>
     </row>
-    <row r="45" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="45" spans="3:3" ht="15.75" customHeight="1">
       <c r="C45" s="16"/>
     </row>
-    <row r="46" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="46" spans="3:3" ht="15.75" customHeight="1">
       <c r="C46" s="16"/>
     </row>
-    <row r="47" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="47" spans="3:3" ht="15.75" customHeight="1">
       <c r="C47" s="16"/>
     </row>
-    <row r="48" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="48" spans="3:3" ht="15.75" customHeight="1">
       <c r="C48" s="16"/>
     </row>
-    <row r="49" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="49" spans="3:3" ht="15.75" customHeight="1">
       <c r="C49" s="16"/>
     </row>
-    <row r="50" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="50" spans="3:3" ht="15.75" customHeight="1">
       <c r="C50" s="16"/>
     </row>
-    <row r="51" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="51" spans="3:3" ht="15.75" customHeight="1">
       <c r="C51" s="16"/>
     </row>
-    <row r="52" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="52" spans="3:3" ht="15.75" customHeight="1">
       <c r="C52" s="16"/>
     </row>
-    <row r="53" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="53" spans="3:3" ht="15.75" customHeight="1">
       <c r="C53" s="16"/>
     </row>
-    <row r="54" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="54" spans="3:3" ht="15.75" customHeight="1">
       <c r="C54" s="16"/>
     </row>
-    <row r="55" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="55" spans="3:3" ht="15.75" customHeight="1">
       <c r="C55" s="16"/>
     </row>
-    <row r="56" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="56" spans="3:3" ht="15.75" customHeight="1">
       <c r="C56" s="16"/>
     </row>
-    <row r="57" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="57" spans="3:3" ht="15.75" customHeight="1">
       <c r="C57" s="16"/>
     </row>
-    <row r="58" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="58" spans="3:3" ht="15.75" customHeight="1">
       <c r="C58" s="16"/>
     </row>
-    <row r="59" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="59" spans="3:3" ht="15.75" customHeight="1">
       <c r="C59" s="16"/>
     </row>
-    <row r="60" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="60" spans="3:3" ht="15.75" customHeight="1">
       <c r="C60" s="16"/>
     </row>
-    <row r="61" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="61" spans="3:3" ht="15.75" customHeight="1">
       <c r="C61" s="16"/>
     </row>
-    <row r="62" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="62" spans="3:3" ht="15.75" customHeight="1">
       <c r="C62" s="16"/>
     </row>
-    <row r="63" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="63" spans="3:3" ht="15.75" customHeight="1">
       <c r="C63" s="16"/>
     </row>
-    <row r="64" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="64" spans="3:3" ht="15.75" customHeight="1">
       <c r="C64" s="16"/>
     </row>
-    <row r="65" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="65" spans="3:3" ht="15.75" customHeight="1">
       <c r="C65" s="16"/>
     </row>
-    <row r="66" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="66" spans="3:3" ht="15.75" customHeight="1">
       <c r="C66" s="16"/>
     </row>
-    <row r="67" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="67" spans="3:3" ht="15.75" customHeight="1">
       <c r="C67" s="16"/>
     </row>
   </sheetData>
@@ -3694,7 +3696,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -3705,15 +3707,15 @@
       <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
-    <col min="2" max="2" width="28.5" customWidth="1"/>
-    <col min="3" max="3" width="24.5" customWidth="1"/>
-    <col min="4" max="6" width="14.5" customWidth="1"/>
+    <col min="2" max="2" width="28.42578125" customWidth="1"/>
+    <col min="3" max="3" width="24.42578125" customWidth="1"/>
+    <col min="4" max="6" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:26" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3755,7 +3757,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:26" ht="15.75" customHeight="1">
       <c r="A2" s="4" t="s">
         <v>8</v>
       </c>
@@ -3764,7 +3766,7 @@
       </c>
       <c r="C2" s="8">
         <f ca="1">NOW()</f>
-        <v>43918.788459606483</v>
+        <v>44010.831003587962</v>
       </c>
       <c r="D2" s="11"/>
       <c r="E2" s="11" t="s">
@@ -3800,7 +3802,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -3811,13 +3813,13 @@
       <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="28.33203125" customWidth="1"/>
-    <col min="2" max="23" width="45.83203125" customWidth="1"/>
+    <col min="1" max="1" width="28.28515625" customWidth="1"/>
+    <col min="2" max="23" width="45.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:23" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>27</v>
       </c>
@@ -3860,7 +3862,7 @@
       <c r="V1" s="10"/>
       <c r="W1" s="10"/>
     </row>
-    <row r="2" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:23" ht="15.75" customHeight="1">
       <c r="A2" s="16" t="s">
         <v>30</v>
       </c>
@@ -3891,7 +3893,7 @@
       <c r="V2" s="16"/>
       <c r="W2" s="16"/>
     </row>
-    <row r="3" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:23" ht="15.75" customHeight="1">
       <c r="A3" s="16" t="s">
         <v>30</v>
       </c>
@@ -3922,7 +3924,7 @@
       <c r="V3" s="16"/>
       <c r="W3" s="16"/>
     </row>
-    <row r="4" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:23" ht="15.75" customHeight="1">
       <c r="A4" s="16"/>
       <c r="B4" s="16"/>
       <c r="C4" s="16"/>
@@ -3947,7 +3949,7 @@
       <c r="V4" s="16"/>
       <c r="W4" s="16"/>
     </row>
-    <row r="5" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:23" ht="15.75" customHeight="1">
       <c r="A5" s="16" t="s">
         <v>73</v>
       </c>
@@ -3978,7 +3980,7 @@
       <c r="V5" s="16"/>
       <c r="W5" s="16"/>
     </row>
-    <row r="6" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:23" ht="15.75" customHeight="1">
       <c r="A6" s="16" t="s">
         <v>73</v>
       </c>
@@ -4009,7 +4011,7 @@
       <c r="V6" s="16"/>
       <c r="W6" s="16"/>
     </row>
-    <row r="7" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:23" ht="15.75" customHeight="1">
       <c r="A7" s="16" t="s">
         <v>73</v>
       </c>
@@ -4040,7 +4042,7 @@
       <c r="V7" s="16"/>
       <c r="W7" s="16"/>
     </row>
-    <row r="8" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:23" ht="15.75" customHeight="1">
       <c r="A8" s="16" t="s">
         <v>73</v>
       </c>
@@ -4071,7 +4073,7 @@
       <c r="V8" s="16"/>
       <c r="W8" s="16"/>
     </row>
-    <row r="9" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:23" ht="15.75" customHeight="1">
       <c r="A9" s="16" t="s">
         <v>73</v>
       </c>
@@ -4102,7 +4104,7 @@
       <c r="V9" s="16"/>
       <c r="W9" s="16"/>
     </row>
-    <row r="10" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:23" ht="15.75" customHeight="1">
       <c r="A10" s="16"/>
       <c r="B10" s="16"/>
       <c r="C10" s="16"/>
@@ -4127,7 +4129,7 @@
       <c r="V10" s="16"/>
       <c r="W10" s="16"/>
     </row>
-    <row r="11" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:23" ht="15.75" customHeight="1">
       <c r="A11" s="16" t="s">
         <v>85</v>
       </c>
@@ -4158,7 +4160,7 @@
       <c r="V11" s="16"/>
       <c r="W11" s="16"/>
     </row>
-    <row r="12" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:23" ht="15.75" customHeight="1">
       <c r="A12" s="16" t="s">
         <v>85</v>
       </c>
@@ -4189,7 +4191,7 @@
       <c r="V12" s="16"/>
       <c r="W12" s="16"/>
     </row>
-    <row r="13" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:23" ht="15.75" customHeight="1">
       <c r="A13" s="16" t="s">
         <v>85</v>
       </c>
@@ -4220,7 +4222,7 @@
       <c r="V13" s="16"/>
       <c r="W13" s="16"/>
     </row>
-    <row r="14" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:23" ht="15.75" customHeight="1">
       <c r="A14" s="16" t="s">
         <v>85</v>
       </c>
@@ -4251,7 +4253,7 @@
       <c r="V14" s="16"/>
       <c r="W14" s="16"/>
     </row>
-    <row r="15" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:23" ht="15.75" customHeight="1">
       <c r="A15" s="16" t="s">
         <v>85</v>
       </c>
@@ -4282,7 +4284,7 @@
       <c r="V15" s="16"/>
       <c r="W15" s="16"/>
     </row>
-    <row r="16" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:23" ht="15.75" customHeight="1">
       <c r="A16" s="16" t="s">
         <v>85</v>
       </c>
@@ -4313,7 +4315,7 @@
       <c r="V16" s="16"/>
       <c r="W16" s="16"/>
     </row>
-    <row r="17" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:23" ht="15.75" customHeight="1">
       <c r="A17" s="16"/>
       <c r="B17" s="16"/>
       <c r="C17" s="16"/>
@@ -4338,7 +4340,7 @@
       <c r="V17" s="16"/>
       <c r="W17" s="16"/>
     </row>
-    <row r="18" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:23" ht="15.75" customHeight="1">
       <c r="A18" s="16" t="s">
         <v>98</v>
       </c>
@@ -4369,7 +4371,7 @@
       <c r="V18" s="16"/>
       <c r="W18" s="16"/>
     </row>
-    <row r="19" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:23" ht="15.75" customHeight="1">
       <c r="A19" s="16" t="s">
         <v>98</v>
       </c>
@@ -4400,7 +4402,7 @@
       <c r="V19" s="16"/>
       <c r="W19" s="16"/>
     </row>
-    <row r="20" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:23" ht="15.75" customHeight="1">
       <c r="A20" s="16" t="s">
         <v>98</v>
       </c>
@@ -4431,7 +4433,7 @@
       <c r="V20" s="16"/>
       <c r="W20" s="16"/>
     </row>
-    <row r="21" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:23" ht="15.75" customHeight="1">
       <c r="A21" s="16" t="s">
         <v>98</v>
       </c>
@@ -4462,7 +4464,7 @@
       <c r="V21" s="16"/>
       <c r="W21" s="16"/>
     </row>
-    <row r="22" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:23" ht="15.75" customHeight="1">
       <c r="A22" s="16" t="s">
         <v>98</v>
       </c>
@@ -4493,7 +4495,7 @@
       <c r="V22" s="16"/>
       <c r="W22" s="16"/>
     </row>
-    <row r="23" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:23" ht="15.75" customHeight="1">
       <c r="A23" s="16" t="s">
         <v>98</v>
       </c>
@@ -4524,7 +4526,7 @@
       <c r="V23" s="16"/>
       <c r="W23" s="16"/>
     </row>
-    <row r="24" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:23" ht="15.75" customHeight="1">
       <c r="A24" s="16"/>
       <c r="B24" s="16"/>
       <c r="C24" s="16"/>
@@ -4549,7 +4551,7 @@
       <c r="V24" s="16"/>
       <c r="W24" s="16"/>
     </row>
-    <row r="25" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:23" ht="15.75" customHeight="1">
       <c r="A25" s="16" t="s">
         <v>101</v>
       </c>
@@ -4580,7 +4582,7 @@
       <c r="V25" s="16"/>
       <c r="W25" s="16"/>
     </row>
-    <row r="26" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:23" ht="15.75" customHeight="1">
       <c r="A26" s="16" t="s">
         <v>101</v>
       </c>
@@ -4611,7 +4613,7 @@
       <c r="V26" s="16"/>
       <c r="W26" s="16"/>
     </row>
-    <row r="27" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:23" ht="15.75" customHeight="1">
       <c r="A27" s="16" t="s">
         <v>101</v>
       </c>
@@ -4642,7 +4644,7 @@
       <c r="V27" s="16"/>
       <c r="W27" s="16"/>
     </row>
-    <row r="28" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:23" ht="15.75" customHeight="1">
       <c r="A28" s="16" t="s">
         <v>101</v>
       </c>
@@ -4673,7 +4675,7 @@
       <c r="V28" s="16"/>
       <c r="W28" s="16"/>
     </row>
-    <row r="29" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:23" ht="15.75" customHeight="1">
       <c r="A29" s="16" t="s">
         <v>101</v>
       </c>
@@ -4704,7 +4706,7 @@
       <c r="V29" s="16"/>
       <c r="W29" s="16"/>
     </row>
-    <row r="30" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:23" ht="15.75" customHeight="1">
       <c r="A30" s="16"/>
       <c r="B30" s="16"/>
       <c r="C30" s="16"/>
@@ -4729,7 +4731,7 @@
       <c r="V30" s="16"/>
       <c r="W30" s="16"/>
     </row>
-    <row r="31" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:23" ht="15.75" customHeight="1">
       <c r="A31" s="16" t="s">
         <v>112</v>
       </c>
@@ -4760,7 +4762,7 @@
       <c r="V31" s="16"/>
       <c r="W31" s="16"/>
     </row>
-    <row r="32" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:23" ht="15.75" customHeight="1">
       <c r="A32" s="16" t="s">
         <v>112</v>
       </c>
@@ -4791,7 +4793,7 @@
       <c r="V32" s="16"/>
       <c r="W32" s="16"/>
     </row>
-    <row r="33" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:23" ht="15.75" customHeight="1">
       <c r="A33" s="16"/>
       <c r="B33" s="16"/>
       <c r="C33" s="16"/>
@@ -4816,7 +4818,7 @@
       <c r="V33" s="16"/>
       <c r="W33" s="16"/>
     </row>
-    <row r="34" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:23" ht="15.75" customHeight="1">
       <c r="A34" t="s">
         <v>115</v>
       </c>
@@ -4828,7 +4830,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="35" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:23" ht="15.75" customHeight="1">
       <c r="A35" t="s">
         <v>115</v>
       </c>
@@ -4840,7 +4842,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="36" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:23" ht="15.75" customHeight="1">
       <c r="A36" t="s">
         <v>115</v>
       </c>
@@ -4852,7 +4854,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="37" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:23" ht="15.75" customHeight="1">
       <c r="A37" t="s">
         <v>115</v>
       </c>
@@ -4864,7 +4866,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="38" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:23" ht="15.75" customHeight="1">
       <c r="A38" t="s">
         <v>115</v>
       </c>
@@ -4876,7 +4878,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="39" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:23" ht="15.75" customHeight="1">
       <c r="A39" t="s">
         <v>115</v>
       </c>
@@ -4888,7 +4890,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="40" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:23" ht="15.75" customHeight="1">
       <c r="A40" t="s">
         <v>115</v>
       </c>
@@ -4900,7 +4902,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="41" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:23" ht="15.75" customHeight="1">
       <c r="A41" t="s">
         <v>115</v>
       </c>
@@ -4912,7 +4914,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="42" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:23" ht="15.75" customHeight="1">
       <c r="A42" t="s">
         <v>115</v>
       </c>
@@ -4924,7 +4926,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="43" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:23" ht="15.75" customHeight="1">
       <c r="A43" t="s">
         <v>115</v>
       </c>
@@ -4935,13 +4937,13 @@
         <v>111</v>
       </c>
     </row>
-    <row r="44" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:23" ht="15.75" customHeight="1">
       <c r="B44" t="str">
         <f t="shared" ref="B44:B47" si="1">SUBSTITUTE(LOWER(SUBSTITUTE(SUBSTITUTE(C44, "(", ""), ")", "")), " ", "_")</f>
         <v/>
       </c>
     </row>
-    <row r="45" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:23" ht="15.75" customHeight="1">
       <c r="A45" t="s">
         <v>137</v>
       </c>
@@ -4953,7 +4955,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="46" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:23" ht="15.75" customHeight="1">
       <c r="A46" t="s">
         <v>137</v>
       </c>
@@ -4965,13 +4967,13 @@
         <v>139</v>
       </c>
     </row>
-    <row r="47" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:23" ht="15.75" customHeight="1">
       <c r="B47" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="48" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:23" ht="15.75" customHeight="1">
       <c r="A48" s="18" t="s">
         <v>140</v>
       </c>
@@ -5002,7 +5004,7 @@
       <c r="V48" s="10"/>
       <c r="W48" s="10"/>
     </row>
-    <row r="49" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:23" ht="15.75" customHeight="1">
       <c r="A49" s="18" t="s">
         <v>140</v>
       </c>
@@ -5033,8 +5035,8 @@
       <c r="V49" s="10"/>
       <c r="W49" s="10"/>
     </row>
-    <row r="50" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="51" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:23" ht="15.75" customHeight="1"/>
+    <row r="51" spans="1:23" ht="15.75" customHeight="1">
       <c r="A51" t="s">
         <v>145</v>
       </c>
@@ -5045,7 +5047,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="52" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:23" ht="15.75" customHeight="1">
       <c r="A52" t="s">
         <v>145</v>
       </c>
@@ -5056,7 +5058,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="53" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:23" ht="15.75" customHeight="1">
       <c r="A53" t="s">
         <v>145</v>
       </c>
@@ -5067,7 +5069,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="54" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:23" ht="15.75" customHeight="1">
       <c r="A54" t="s">
         <v>145</v>
       </c>
@@ -5078,7 +5080,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="55" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:23" ht="15.75" customHeight="1">
       <c r="A55" t="s">
         <v>145</v>
       </c>
@@ -5089,7 +5091,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="56" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:23" ht="15.75" customHeight="1">
       <c r="A56" t="s">
         <v>145</v>
       </c>
@@ -5100,8 +5102,8 @@
         <v>111</v>
       </c>
     </row>
-    <row r="57" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="58" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:23" ht="15.75" customHeight="1"/>
+    <row r="58" spans="1:23" ht="15.75" customHeight="1">
       <c r="A58" s="18" t="s">
         <v>156</v>
       </c>
@@ -5112,7 +5114,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="59" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:23" ht="15.75" customHeight="1">
       <c r="A59" s="18" t="s">
         <v>156</v>
       </c>
@@ -5123,7 +5125,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="60" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:23" ht="15.75" customHeight="1">
       <c r="A60" s="18" t="s">
         <v>156</v>
       </c>
@@ -5134,7 +5136,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="61" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:23" ht="15.75" customHeight="1">
       <c r="A61" s="18" t="s">
         <v>156</v>
       </c>
@@ -5145,8 +5147,8 @@
         <v>111</v>
       </c>
     </row>
-    <row r="62" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="63" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:23" ht="15.75" customHeight="1"/>
+    <row r="63" spans="1:23" ht="15.75" customHeight="1">
       <c r="A63" s="10" t="s">
         <v>165</v>
       </c>
@@ -5157,7 +5159,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="64" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:23" ht="15.75" customHeight="1">
       <c r="A64" s="10" t="s">
         <v>165</v>
       </c>
@@ -5168,7 +5170,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="65" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:3" ht="15.75" customHeight="1">
       <c r="A65" s="10" t="s">
         <v>165</v>
       </c>
@@ -5179,7 +5181,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="66" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:3" ht="15.75" customHeight="1">
       <c r="A66" s="10" t="s">
         <v>165</v>
       </c>
@@ -5190,7 +5192,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="67" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="67" spans="1:3" ht="15.75" customHeight="1">
       <c r="A67" s="10" t="s">
         <v>165</v>
       </c>
@@ -5201,8 +5203,8 @@
         <v>175</v>
       </c>
     </row>
-    <row r="68" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="69" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="68" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="69" spans="1:3" ht="15.75" customHeight="1">
       <c r="A69" t="s">
         <v>176</v>
       </c>
@@ -5213,7 +5215,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="70" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:3" ht="15.75" customHeight="1">
       <c r="A70" t="s">
         <v>176</v>
       </c>
@@ -5224,8 +5226,8 @@
         <v>181</v>
       </c>
     </row>
-    <row r="71" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="72" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="71" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="72" spans="1:3" ht="15.75" customHeight="1">
       <c r="A72" t="s">
         <v>184</v>
       </c>
@@ -5236,7 +5238,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="73" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="73" spans="1:3" ht="15.75" customHeight="1">
       <c r="A73" t="s">
         <v>184</v>
       </c>
@@ -5247,7 +5249,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="74" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="74" spans="1:3" ht="15.75" customHeight="1">
       <c r="A74" t="s">
         <v>184</v>
       </c>
@@ -5258,932 +5260,932 @@
         <v>111</v>
       </c>
     </row>
-    <row r="75" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="76" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="77" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="78" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="79" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="80" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="81" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="82" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="83" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="84" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="85" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="86" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="87" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="88" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="89" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="90" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="91" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="92" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="93" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="94" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="95" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="96" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="97" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="98" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="99" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="100" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="101" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="102" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="103" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="104" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="105" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="106" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="107" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="108" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="109" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="110" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="111" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="112" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="113" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="114" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="115" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="116" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="117" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="118" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="119" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="120" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="121" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="122" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="123" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="124" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="125" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="126" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="127" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="128" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="129" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="130" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="131" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="132" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="133" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="134" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="135" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="136" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="137" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="138" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="139" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="140" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="141" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="142" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="143" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="144" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="145" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="146" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="147" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="148" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="149" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="150" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="151" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="152" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="153" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="154" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="155" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="156" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="157" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="158" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="159" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="160" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="161" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="162" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="163" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="164" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="165" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="166" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="167" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="168" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="169" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="170" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="171" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="172" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="173" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="174" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="175" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="176" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="177" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="178" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="179" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="180" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="181" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="182" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="183" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="184" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="185" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="186" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="187" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="188" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="189" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="190" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="191" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="192" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="193" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="194" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="195" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="196" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="197" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="198" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="199" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="200" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="201" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="202" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="203" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="204" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="205" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="206" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="207" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="208" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="209" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="210" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="211" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="212" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="213" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="214" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="215" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="216" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="217" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="218" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="219" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="220" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="221" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="222" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="223" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="224" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="225" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="226" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="227" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="228" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="229" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="230" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="231" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="232" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="233" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="234" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="235" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="236" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="237" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="238" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="239" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="240" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="241" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="242" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="243" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="244" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="245" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="246" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="247" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="248" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="249" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="250" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="251" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="252" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="253" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="254" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="255" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="256" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="257" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="258" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="259" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="260" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="261" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="262" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="263" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="264" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="265" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="266" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="267" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="268" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="269" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="270" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="271" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="272" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="273" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="274" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="275" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="276" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="277" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="278" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="279" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="280" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="281" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="282" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="283" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="284" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="285" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="286" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="287" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="288" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="289" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="290" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="291" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="292" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="293" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="294" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="295" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="296" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="297" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="298" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="299" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="300" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="301" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="302" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="303" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="304" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="305" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="306" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="307" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="308" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="309" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="310" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="311" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="312" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="313" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="314" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="315" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="316" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="317" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="318" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="319" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="320" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="321" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="322" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="323" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="324" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="325" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="326" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="327" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="328" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="329" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="330" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="331" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="332" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="333" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="334" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="335" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="336" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="337" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="338" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="339" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="340" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="341" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="342" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="343" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="344" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="345" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="346" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="347" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="348" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="349" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="350" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="351" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="352" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="353" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="354" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="355" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="356" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="357" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="358" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="359" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="360" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="361" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="362" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="363" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="364" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="365" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="366" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="367" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="368" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="369" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="370" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="371" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="372" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="373" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="374" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="375" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="376" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="377" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="378" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="379" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="380" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="381" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="382" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="383" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="384" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="385" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="386" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="387" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="388" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="389" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="390" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="391" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="392" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="393" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="394" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="395" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="396" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="397" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="398" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="399" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="400" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="401" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="402" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="403" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="404" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="405" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="406" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="407" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="408" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="409" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="410" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="411" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="412" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="413" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="414" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="415" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="416" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="417" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="418" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="419" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="420" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="421" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="422" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="423" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="424" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="425" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="426" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="427" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="428" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="429" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="430" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="431" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="432" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="433" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="434" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="435" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="436" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="437" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="438" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="439" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="440" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="441" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="442" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="443" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="444" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="445" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="446" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="447" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="448" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="449" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="450" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="451" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="452" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="453" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="454" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="455" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="456" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="457" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="458" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="459" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="460" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="461" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="462" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="463" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="464" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="465" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="466" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="467" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="468" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="469" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="470" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="471" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="472" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="473" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="474" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="475" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="476" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="477" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="478" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="479" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="480" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="481" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="482" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="483" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="484" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="485" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="486" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="487" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="488" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="489" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="490" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="491" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="492" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="493" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="494" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="495" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="496" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="497" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="498" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="499" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="500" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="501" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="502" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="503" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="504" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="505" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="506" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="507" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="508" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="509" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="510" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="511" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="512" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="513" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="514" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="515" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="516" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="517" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="518" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="519" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="520" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="521" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="522" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="523" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="524" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="525" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="526" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="527" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="528" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="529" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="530" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="531" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="532" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="533" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="534" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="535" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="536" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="537" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="538" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="539" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="540" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="541" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="542" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="543" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="544" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="545" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="546" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="547" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="548" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="549" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="550" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="551" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="552" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="553" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="554" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="555" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="556" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="557" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="558" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="559" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="560" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="561" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="562" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="563" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="564" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="565" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="566" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="567" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="568" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="569" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="570" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="571" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="572" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="573" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="574" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="575" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="576" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="577" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="578" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="579" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="580" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="581" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="582" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="583" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="584" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="585" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="586" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="587" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="588" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="589" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="590" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="591" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="592" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="593" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="594" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="595" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="596" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="597" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="598" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="599" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="600" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="601" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="602" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="603" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="604" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="605" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="606" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="607" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="608" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="609" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="610" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="611" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="612" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="613" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="614" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="615" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="616" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="617" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="618" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="619" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="620" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="621" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="622" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="623" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="624" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="625" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="626" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="627" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="628" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="629" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="630" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="631" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="632" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="633" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="634" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="635" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="636" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="637" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="638" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="639" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="640" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="641" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="642" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="643" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="644" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="645" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="646" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="647" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="648" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="649" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="650" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="651" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="652" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="653" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="654" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="655" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="656" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="657" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="658" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="659" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="660" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="661" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="662" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="663" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="664" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="665" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="666" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="667" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="668" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="669" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="670" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="671" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="672" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="673" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="674" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="675" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="676" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="677" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="678" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="679" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="680" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="681" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="682" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="683" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="684" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="685" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="686" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="687" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="688" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="689" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="690" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="691" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="692" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="693" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="694" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="695" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="696" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="697" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="698" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="699" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="700" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="701" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="702" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="703" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="704" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="705" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="706" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="707" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="708" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="709" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="710" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="711" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="712" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="713" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="714" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="715" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="716" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="717" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="718" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="719" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="720" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="721" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="722" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="723" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="724" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="725" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="726" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="727" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="728" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="729" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="730" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="731" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="732" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="733" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="734" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="735" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="736" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="737" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="738" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="739" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="740" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="741" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="742" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="743" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="744" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="745" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="746" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="747" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="748" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="749" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="750" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="751" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="752" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="753" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="754" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="755" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="756" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="757" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="758" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="759" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="760" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="761" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="762" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="763" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="764" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="765" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="766" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="767" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="768" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="769" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="770" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="771" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="772" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="773" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="774" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="775" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="776" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="777" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="778" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="779" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="780" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="781" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="782" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="783" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="784" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="785" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="786" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="787" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="788" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="789" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="790" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="791" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="792" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="793" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="794" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="795" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="796" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="797" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="798" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="799" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="800" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="801" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="802" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="803" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="804" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="805" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="806" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="807" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="808" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="809" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="810" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="811" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="812" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="813" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="814" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="815" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="816" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="817" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="818" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="819" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="820" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="821" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="822" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="823" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="824" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="825" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="826" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="827" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="828" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="829" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="830" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="831" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="832" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="833" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="834" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="835" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="836" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="837" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="838" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="839" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="840" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="841" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="842" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="843" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="844" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="845" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="846" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="847" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="848" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="849" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="850" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="851" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="852" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="853" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="854" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="855" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="856" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="857" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="858" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="859" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="860" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="861" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="862" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="863" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="864" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="865" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="866" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="867" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="868" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="869" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="870" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="871" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="872" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="873" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="874" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="875" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="876" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="877" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="878" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="879" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="880" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="881" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="882" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="883" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="884" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="885" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="886" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="887" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="888" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="889" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="890" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="891" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="892" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="893" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="894" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="895" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="896" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="897" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="898" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="899" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="900" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="901" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="902" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="903" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="904" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="905" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="906" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="907" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="908" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="909" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="910" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="911" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="912" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="913" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="914" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="915" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="916" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="917" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="918" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="919" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="920" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="921" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="922" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="923" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="924" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="925" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="926" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="927" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="928" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="929" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="930" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="931" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="932" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="933" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="934" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="935" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="936" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="937" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="938" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="939" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="940" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="941" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="942" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="943" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="944" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="945" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="946" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="947" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="948" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="949" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="950" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="951" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="952" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="953" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="954" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="955" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="956" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="957" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="958" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="959" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="960" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="961" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="962" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="963" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="964" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="965" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="966" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="967" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="968" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="969" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="970" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="971" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="972" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="973" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="974" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="975" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="976" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="977" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="978" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="979" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="980" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="981" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="982" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="983" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="984" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="985" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="986" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="987" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="988" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="989" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="990" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="991" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="992" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="993" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="994" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="995" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="996" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="997" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="75" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="76" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="77" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="78" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="79" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="80" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="81" ht="15.75" customHeight="1"/>
+    <row r="82" ht="15.75" customHeight="1"/>
+    <row r="83" ht="15.75" customHeight="1"/>
+    <row r="84" ht="15.75" customHeight="1"/>
+    <row r="85" ht="15.75" customHeight="1"/>
+    <row r="86" ht="15.75" customHeight="1"/>
+    <row r="87" ht="15.75" customHeight="1"/>
+    <row r="88" ht="15.75" customHeight="1"/>
+    <row r="89" ht="15.75" customHeight="1"/>
+    <row r="90" ht="15.75" customHeight="1"/>
+    <row r="91" ht="15.75" customHeight="1"/>
+    <row r="92" ht="15.75" customHeight="1"/>
+    <row r="93" ht="15.75" customHeight="1"/>
+    <row r="94" ht="15.75" customHeight="1"/>
+    <row r="95" ht="15.75" customHeight="1"/>
+    <row r="96" ht="15.75" customHeight="1"/>
+    <row r="97" ht="15.75" customHeight="1"/>
+    <row r="98" ht="15.75" customHeight="1"/>
+    <row r="99" ht="15.75" customHeight="1"/>
+    <row r="100" ht="15.75" customHeight="1"/>
+    <row r="101" ht="15.75" customHeight="1"/>
+    <row r="102" ht="15.75" customHeight="1"/>
+    <row r="103" ht="15.75" customHeight="1"/>
+    <row r="104" ht="15.75" customHeight="1"/>
+    <row r="105" ht="15.75" customHeight="1"/>
+    <row r="106" ht="15.75" customHeight="1"/>
+    <row r="107" ht="15.75" customHeight="1"/>
+    <row r="108" ht="15.75" customHeight="1"/>
+    <row r="109" ht="15.75" customHeight="1"/>
+    <row r="110" ht="15.75" customHeight="1"/>
+    <row r="111" ht="15.75" customHeight="1"/>
+    <row r="112" ht="15.75" customHeight="1"/>
+    <row r="113" ht="15.75" customHeight="1"/>
+    <row r="114" ht="15.75" customHeight="1"/>
+    <row r="115" ht="15.75" customHeight="1"/>
+    <row r="116" ht="15.75" customHeight="1"/>
+    <row r="117" ht="15.75" customHeight="1"/>
+    <row r="118" ht="15.75" customHeight="1"/>
+    <row r="119" ht="15.75" customHeight="1"/>
+    <row r="120" ht="15.75" customHeight="1"/>
+    <row r="121" ht="15.75" customHeight="1"/>
+    <row r="122" ht="15.75" customHeight="1"/>
+    <row r="123" ht="15.75" customHeight="1"/>
+    <row r="124" ht="15.75" customHeight="1"/>
+    <row r="125" ht="15.75" customHeight="1"/>
+    <row r="126" ht="15.75" customHeight="1"/>
+    <row r="127" ht="15.75" customHeight="1"/>
+    <row r="128" ht="15.75" customHeight="1"/>
+    <row r="129" ht="15.75" customHeight="1"/>
+    <row r="130" ht="15.75" customHeight="1"/>
+    <row r="131" ht="15.75" customHeight="1"/>
+    <row r="132" ht="15.75" customHeight="1"/>
+    <row r="133" ht="15.75" customHeight="1"/>
+    <row r="134" ht="15.75" customHeight="1"/>
+    <row r="135" ht="15.75" customHeight="1"/>
+    <row r="136" ht="15.75" customHeight="1"/>
+    <row r="137" ht="15.75" customHeight="1"/>
+    <row r="138" ht="15.75" customHeight="1"/>
+    <row r="139" ht="15.75" customHeight="1"/>
+    <row r="140" ht="15.75" customHeight="1"/>
+    <row r="141" ht="15.75" customHeight="1"/>
+    <row r="142" ht="15.75" customHeight="1"/>
+    <row r="143" ht="15.75" customHeight="1"/>
+    <row r="144" ht="15.75" customHeight="1"/>
+    <row r="145" ht="15.75" customHeight="1"/>
+    <row r="146" ht="15.75" customHeight="1"/>
+    <row r="147" ht="15.75" customHeight="1"/>
+    <row r="148" ht="15.75" customHeight="1"/>
+    <row r="149" ht="15.75" customHeight="1"/>
+    <row r="150" ht="15.75" customHeight="1"/>
+    <row r="151" ht="15.75" customHeight="1"/>
+    <row r="152" ht="15.75" customHeight="1"/>
+    <row r="153" ht="15.75" customHeight="1"/>
+    <row r="154" ht="15.75" customHeight="1"/>
+    <row r="155" ht="15.75" customHeight="1"/>
+    <row r="156" ht="15.75" customHeight="1"/>
+    <row r="157" ht="15.75" customHeight="1"/>
+    <row r="158" ht="15.75" customHeight="1"/>
+    <row r="159" ht="15.75" customHeight="1"/>
+    <row r="160" ht="15.75" customHeight="1"/>
+    <row r="161" ht="15.75" customHeight="1"/>
+    <row r="162" ht="15.75" customHeight="1"/>
+    <row r="163" ht="15.75" customHeight="1"/>
+    <row r="164" ht="15.75" customHeight="1"/>
+    <row r="165" ht="15.75" customHeight="1"/>
+    <row r="166" ht="15.75" customHeight="1"/>
+    <row r="167" ht="15.75" customHeight="1"/>
+    <row r="168" ht="15.75" customHeight="1"/>
+    <row r="169" ht="15.75" customHeight="1"/>
+    <row r="170" ht="15.75" customHeight="1"/>
+    <row r="171" ht="15.75" customHeight="1"/>
+    <row r="172" ht="15.75" customHeight="1"/>
+    <row r="173" ht="15.75" customHeight="1"/>
+    <row r="174" ht="15.75" customHeight="1"/>
+    <row r="175" ht="15.75" customHeight="1"/>
+    <row r="176" ht="15.75" customHeight="1"/>
+    <row r="177" ht="15.75" customHeight="1"/>
+    <row r="178" ht="15.75" customHeight="1"/>
+    <row r="179" ht="15.75" customHeight="1"/>
+    <row r="180" ht="15.75" customHeight="1"/>
+    <row r="181" ht="15.75" customHeight="1"/>
+    <row r="182" ht="15.75" customHeight="1"/>
+    <row r="183" ht="15.75" customHeight="1"/>
+    <row r="184" ht="15.75" customHeight="1"/>
+    <row r="185" ht="15.75" customHeight="1"/>
+    <row r="186" ht="15.75" customHeight="1"/>
+    <row r="187" ht="15.75" customHeight="1"/>
+    <row r="188" ht="15.75" customHeight="1"/>
+    <row r="189" ht="15.75" customHeight="1"/>
+    <row r="190" ht="15.75" customHeight="1"/>
+    <row r="191" ht="15.75" customHeight="1"/>
+    <row r="192" ht="15.75" customHeight="1"/>
+    <row r="193" ht="15.75" customHeight="1"/>
+    <row r="194" ht="15.75" customHeight="1"/>
+    <row r="195" ht="15.75" customHeight="1"/>
+    <row r="196" ht="15.75" customHeight="1"/>
+    <row r="197" ht="15.75" customHeight="1"/>
+    <row r="198" ht="15.75" customHeight="1"/>
+    <row r="199" ht="15.75" customHeight="1"/>
+    <row r="200" ht="15.75" customHeight="1"/>
+    <row r="201" ht="15.75" customHeight="1"/>
+    <row r="202" ht="15.75" customHeight="1"/>
+    <row r="203" ht="15.75" customHeight="1"/>
+    <row r="204" ht="15.75" customHeight="1"/>
+    <row r="205" ht="15.75" customHeight="1"/>
+    <row r="206" ht="15.75" customHeight="1"/>
+    <row r="207" ht="15.75" customHeight="1"/>
+    <row r="208" ht="15.75" customHeight="1"/>
+    <row r="209" ht="15.75" customHeight="1"/>
+    <row r="210" ht="15.75" customHeight="1"/>
+    <row r="211" ht="15.75" customHeight="1"/>
+    <row r="212" ht="15.75" customHeight="1"/>
+    <row r="213" ht="15.75" customHeight="1"/>
+    <row r="214" ht="15.75" customHeight="1"/>
+    <row r="215" ht="15.75" customHeight="1"/>
+    <row r="216" ht="15.75" customHeight="1"/>
+    <row r="217" ht="15.75" customHeight="1"/>
+    <row r="218" ht="15.75" customHeight="1"/>
+    <row r="219" ht="15.75" customHeight="1"/>
+    <row r="220" ht="15.75" customHeight="1"/>
+    <row r="221" ht="15.75" customHeight="1"/>
+    <row r="222" ht="15.75" customHeight="1"/>
+    <row r="223" ht="15.75" customHeight="1"/>
+    <row r="224" ht="15.75" customHeight="1"/>
+    <row r="225" ht="15.75" customHeight="1"/>
+    <row r="226" ht="15.75" customHeight="1"/>
+    <row r="227" ht="15.75" customHeight="1"/>
+    <row r="228" ht="15.75" customHeight="1"/>
+    <row r="229" ht="15.75" customHeight="1"/>
+    <row r="230" ht="15.75" customHeight="1"/>
+    <row r="231" ht="15.75" customHeight="1"/>
+    <row r="232" ht="15.75" customHeight="1"/>
+    <row r="233" ht="15.75" customHeight="1"/>
+    <row r="234" ht="15.75" customHeight="1"/>
+    <row r="235" ht="15.75" customHeight="1"/>
+    <row r="236" ht="15.75" customHeight="1"/>
+    <row r="237" ht="15.75" customHeight="1"/>
+    <row r="238" ht="15.75" customHeight="1"/>
+    <row r="239" ht="15.75" customHeight="1"/>
+    <row r="240" ht="15.75" customHeight="1"/>
+    <row r="241" ht="15.75" customHeight="1"/>
+    <row r="242" ht="15.75" customHeight="1"/>
+    <row r="243" ht="15.75" customHeight="1"/>
+    <row r="244" ht="15.75" customHeight="1"/>
+    <row r="245" ht="15.75" customHeight="1"/>
+    <row r="246" ht="15.75" customHeight="1"/>
+    <row r="247" ht="15.75" customHeight="1"/>
+    <row r="248" ht="15.75" customHeight="1"/>
+    <row r="249" ht="15.75" customHeight="1"/>
+    <row r="250" ht="15.75" customHeight="1"/>
+    <row r="251" ht="15.75" customHeight="1"/>
+    <row r="252" ht="15.75" customHeight="1"/>
+    <row r="253" ht="15.75" customHeight="1"/>
+    <row r="254" ht="15.75" customHeight="1"/>
+    <row r="255" ht="15.75" customHeight="1"/>
+    <row r="256" ht="15.75" customHeight="1"/>
+    <row r="257" ht="15.75" customHeight="1"/>
+    <row r="258" ht="15.75" customHeight="1"/>
+    <row r="259" ht="15.75" customHeight="1"/>
+    <row r="260" ht="15.75" customHeight="1"/>
+    <row r="261" ht="15.75" customHeight="1"/>
+    <row r="262" ht="15.75" customHeight="1"/>
+    <row r="263" ht="15.75" customHeight="1"/>
+    <row r="264" ht="15.75" customHeight="1"/>
+    <row r="265" ht="15.75" customHeight="1"/>
+    <row r="266" ht="15.75" customHeight="1"/>
+    <row r="267" ht="15.75" customHeight="1"/>
+    <row r="268" ht="15.75" customHeight="1"/>
+    <row r="269" ht="15.75" customHeight="1"/>
+    <row r="270" ht="15.75" customHeight="1"/>
+    <row r="271" ht="15.75" customHeight="1"/>
+    <row r="272" ht="15.75" customHeight="1"/>
+    <row r="273" ht="15.75" customHeight="1"/>
+    <row r="274" ht="15.75" customHeight="1"/>
+    <row r="275" ht="15.75" customHeight="1"/>
+    <row r="276" ht="15.75" customHeight="1"/>
+    <row r="277" ht="15.75" customHeight="1"/>
+    <row r="278" ht="15.75" customHeight="1"/>
+    <row r="279" ht="15.75" customHeight="1"/>
+    <row r="280" ht="15.75" customHeight="1"/>
+    <row r="281" ht="15.75" customHeight="1"/>
+    <row r="282" ht="15.75" customHeight="1"/>
+    <row r="283" ht="15.75" customHeight="1"/>
+    <row r="284" ht="15.75" customHeight="1"/>
+    <row r="285" ht="15.75" customHeight="1"/>
+    <row r="286" ht="15.75" customHeight="1"/>
+    <row r="287" ht="15.75" customHeight="1"/>
+    <row r="288" ht="15.75" customHeight="1"/>
+    <row r="289" ht="15.75" customHeight="1"/>
+    <row r="290" ht="15.75" customHeight="1"/>
+    <row r="291" ht="15.75" customHeight="1"/>
+    <row r="292" ht="15.75" customHeight="1"/>
+    <row r="293" ht="15.75" customHeight="1"/>
+    <row r="294" ht="15.75" customHeight="1"/>
+    <row r="295" ht="15.75" customHeight="1"/>
+    <row r="296" ht="15.75" customHeight="1"/>
+    <row r="297" ht="15.75" customHeight="1"/>
+    <row r="298" ht="15.75" customHeight="1"/>
+    <row r="299" ht="15.75" customHeight="1"/>
+    <row r="300" ht="15.75" customHeight="1"/>
+    <row r="301" ht="15.75" customHeight="1"/>
+    <row r="302" ht="15.75" customHeight="1"/>
+    <row r="303" ht="15.75" customHeight="1"/>
+    <row r="304" ht="15.75" customHeight="1"/>
+    <row r="305" ht="15.75" customHeight="1"/>
+    <row r="306" ht="15.75" customHeight="1"/>
+    <row r="307" ht="15.75" customHeight="1"/>
+    <row r="308" ht="15.75" customHeight="1"/>
+    <row r="309" ht="15.75" customHeight="1"/>
+    <row r="310" ht="15.75" customHeight="1"/>
+    <row r="311" ht="15.75" customHeight="1"/>
+    <row r="312" ht="15.75" customHeight="1"/>
+    <row r="313" ht="15.75" customHeight="1"/>
+    <row r="314" ht="15.75" customHeight="1"/>
+    <row r="315" ht="15.75" customHeight="1"/>
+    <row r="316" ht="15.75" customHeight="1"/>
+    <row r="317" ht="15.75" customHeight="1"/>
+    <row r="318" ht="15.75" customHeight="1"/>
+    <row r="319" ht="15.75" customHeight="1"/>
+    <row r="320" ht="15.75" customHeight="1"/>
+    <row r="321" ht="15.75" customHeight="1"/>
+    <row r="322" ht="15.75" customHeight="1"/>
+    <row r="323" ht="15.75" customHeight="1"/>
+    <row r="324" ht="15.75" customHeight="1"/>
+    <row r="325" ht="15.75" customHeight="1"/>
+    <row r="326" ht="15.75" customHeight="1"/>
+    <row r="327" ht="15.75" customHeight="1"/>
+    <row r="328" ht="15.75" customHeight="1"/>
+    <row r="329" ht="15.75" customHeight="1"/>
+    <row r="330" ht="15.75" customHeight="1"/>
+    <row r="331" ht="15.75" customHeight="1"/>
+    <row r="332" ht="15.75" customHeight="1"/>
+    <row r="333" ht="15.75" customHeight="1"/>
+    <row r="334" ht="15.75" customHeight="1"/>
+    <row r="335" ht="15.75" customHeight="1"/>
+    <row r="336" ht="15.75" customHeight="1"/>
+    <row r="337" ht="15.75" customHeight="1"/>
+    <row r="338" ht="15.75" customHeight="1"/>
+    <row r="339" ht="15.75" customHeight="1"/>
+    <row r="340" ht="15.75" customHeight="1"/>
+    <row r="341" ht="15.75" customHeight="1"/>
+    <row r="342" ht="15.75" customHeight="1"/>
+    <row r="343" ht="15.75" customHeight="1"/>
+    <row r="344" ht="15.75" customHeight="1"/>
+    <row r="345" ht="15.75" customHeight="1"/>
+    <row r="346" ht="15.75" customHeight="1"/>
+    <row r="347" ht="15.75" customHeight="1"/>
+    <row r="348" ht="15.75" customHeight="1"/>
+    <row r="349" ht="15.75" customHeight="1"/>
+    <row r="350" ht="15.75" customHeight="1"/>
+    <row r="351" ht="15.75" customHeight="1"/>
+    <row r="352" ht="15.75" customHeight="1"/>
+    <row r="353" ht="15.75" customHeight="1"/>
+    <row r="354" ht="15.75" customHeight="1"/>
+    <row r="355" ht="15.75" customHeight="1"/>
+    <row r="356" ht="15.75" customHeight="1"/>
+    <row r="357" ht="15.75" customHeight="1"/>
+    <row r="358" ht="15.75" customHeight="1"/>
+    <row r="359" ht="15.75" customHeight="1"/>
+    <row r="360" ht="15.75" customHeight="1"/>
+    <row r="361" ht="15.75" customHeight="1"/>
+    <row r="362" ht="15.75" customHeight="1"/>
+    <row r="363" ht="15.75" customHeight="1"/>
+    <row r="364" ht="15.75" customHeight="1"/>
+    <row r="365" ht="15.75" customHeight="1"/>
+    <row r="366" ht="15.75" customHeight="1"/>
+    <row r="367" ht="15.75" customHeight="1"/>
+    <row r="368" ht="15.75" customHeight="1"/>
+    <row r="369" ht="15.75" customHeight="1"/>
+    <row r="370" ht="15.75" customHeight="1"/>
+    <row r="371" ht="15.75" customHeight="1"/>
+    <row r="372" ht="15.75" customHeight="1"/>
+    <row r="373" ht="15.75" customHeight="1"/>
+    <row r="374" ht="15.75" customHeight="1"/>
+    <row r="375" ht="15.75" customHeight="1"/>
+    <row r="376" ht="15.75" customHeight="1"/>
+    <row r="377" ht="15.75" customHeight="1"/>
+    <row r="378" ht="15.75" customHeight="1"/>
+    <row r="379" ht="15.75" customHeight="1"/>
+    <row r="380" ht="15.75" customHeight="1"/>
+    <row r="381" ht="15.75" customHeight="1"/>
+    <row r="382" ht="15.75" customHeight="1"/>
+    <row r="383" ht="15.75" customHeight="1"/>
+    <row r="384" ht="15.75" customHeight="1"/>
+    <row r="385" ht="15.75" customHeight="1"/>
+    <row r="386" ht="15.75" customHeight="1"/>
+    <row r="387" ht="15.75" customHeight="1"/>
+    <row r="388" ht="15.75" customHeight="1"/>
+    <row r="389" ht="15.75" customHeight="1"/>
+    <row r="390" ht="15.75" customHeight="1"/>
+    <row r="391" ht="15.75" customHeight="1"/>
+    <row r="392" ht="15.75" customHeight="1"/>
+    <row r="393" ht="15.75" customHeight="1"/>
+    <row r="394" ht="15.75" customHeight="1"/>
+    <row r="395" ht="15.75" customHeight="1"/>
+    <row r="396" ht="15.75" customHeight="1"/>
+    <row r="397" ht="15.75" customHeight="1"/>
+    <row r="398" ht="15.75" customHeight="1"/>
+    <row r="399" ht="15.75" customHeight="1"/>
+    <row r="400" ht="15.75" customHeight="1"/>
+    <row r="401" ht="15.75" customHeight="1"/>
+    <row r="402" ht="15.75" customHeight="1"/>
+    <row r="403" ht="15.75" customHeight="1"/>
+    <row r="404" ht="15.75" customHeight="1"/>
+    <row r="405" ht="15.75" customHeight="1"/>
+    <row r="406" ht="15.75" customHeight="1"/>
+    <row r="407" ht="15.75" customHeight="1"/>
+    <row r="408" ht="15.75" customHeight="1"/>
+    <row r="409" ht="15.75" customHeight="1"/>
+    <row r="410" ht="15.75" customHeight="1"/>
+    <row r="411" ht="15.75" customHeight="1"/>
+    <row r="412" ht="15.75" customHeight="1"/>
+    <row r="413" ht="15.75" customHeight="1"/>
+    <row r="414" ht="15.75" customHeight="1"/>
+    <row r="415" ht="15.75" customHeight="1"/>
+    <row r="416" ht="15.75" customHeight="1"/>
+    <row r="417" ht="15.75" customHeight="1"/>
+    <row r="418" ht="15.75" customHeight="1"/>
+    <row r="419" ht="15.75" customHeight="1"/>
+    <row r="420" ht="15.75" customHeight="1"/>
+    <row r="421" ht="15.75" customHeight="1"/>
+    <row r="422" ht="15.75" customHeight="1"/>
+    <row r="423" ht="15.75" customHeight="1"/>
+    <row r="424" ht="15.75" customHeight="1"/>
+    <row r="425" ht="15.75" customHeight="1"/>
+    <row r="426" ht="15.75" customHeight="1"/>
+    <row r="427" ht="15.75" customHeight="1"/>
+    <row r="428" ht="15.75" customHeight="1"/>
+    <row r="429" ht="15.75" customHeight="1"/>
+    <row r="430" ht="15.75" customHeight="1"/>
+    <row r="431" ht="15.75" customHeight="1"/>
+    <row r="432" ht="15.75" customHeight="1"/>
+    <row r="433" ht="15.75" customHeight="1"/>
+    <row r="434" ht="15.75" customHeight="1"/>
+    <row r="435" ht="15.75" customHeight="1"/>
+    <row r="436" ht="15.75" customHeight="1"/>
+    <row r="437" ht="15.75" customHeight="1"/>
+    <row r="438" ht="15.75" customHeight="1"/>
+    <row r="439" ht="15.75" customHeight="1"/>
+    <row r="440" ht="15.75" customHeight="1"/>
+    <row r="441" ht="15.75" customHeight="1"/>
+    <row r="442" ht="15.75" customHeight="1"/>
+    <row r="443" ht="15.75" customHeight="1"/>
+    <row r="444" ht="15.75" customHeight="1"/>
+    <row r="445" ht="15.75" customHeight="1"/>
+    <row r="446" ht="15.75" customHeight="1"/>
+    <row r="447" ht="15.75" customHeight="1"/>
+    <row r="448" ht="15.75" customHeight="1"/>
+    <row r="449" ht="15.75" customHeight="1"/>
+    <row r="450" ht="15.75" customHeight="1"/>
+    <row r="451" ht="15.75" customHeight="1"/>
+    <row r="452" ht="15.75" customHeight="1"/>
+    <row r="453" ht="15.75" customHeight="1"/>
+    <row r="454" ht="15.75" customHeight="1"/>
+    <row r="455" ht="15.75" customHeight="1"/>
+    <row r="456" ht="15.75" customHeight="1"/>
+    <row r="457" ht="15.75" customHeight="1"/>
+    <row r="458" ht="15.75" customHeight="1"/>
+    <row r="459" ht="15.75" customHeight="1"/>
+    <row r="460" ht="15.75" customHeight="1"/>
+    <row r="461" ht="15.75" customHeight="1"/>
+    <row r="462" ht="15.75" customHeight="1"/>
+    <row r="463" ht="15.75" customHeight="1"/>
+    <row r="464" ht="15.75" customHeight="1"/>
+    <row r="465" ht="15.75" customHeight="1"/>
+    <row r="466" ht="15.75" customHeight="1"/>
+    <row r="467" ht="15.75" customHeight="1"/>
+    <row r="468" ht="15.75" customHeight="1"/>
+    <row r="469" ht="15.75" customHeight="1"/>
+    <row r="470" ht="15.75" customHeight="1"/>
+    <row r="471" ht="15.75" customHeight="1"/>
+    <row r="472" ht="15.75" customHeight="1"/>
+    <row r="473" ht="15.75" customHeight="1"/>
+    <row r="474" ht="15.75" customHeight="1"/>
+    <row r="475" ht="15.75" customHeight="1"/>
+    <row r="476" ht="15.75" customHeight="1"/>
+    <row r="477" ht="15.75" customHeight="1"/>
+    <row r="478" ht="15.75" customHeight="1"/>
+    <row r="479" ht="15.75" customHeight="1"/>
+    <row r="480" ht="15.75" customHeight="1"/>
+    <row r="481" ht="15.75" customHeight="1"/>
+    <row r="482" ht="15.75" customHeight="1"/>
+    <row r="483" ht="15.75" customHeight="1"/>
+    <row r="484" ht="15.75" customHeight="1"/>
+    <row r="485" ht="15.75" customHeight="1"/>
+    <row r="486" ht="15.75" customHeight="1"/>
+    <row r="487" ht="15.75" customHeight="1"/>
+    <row r="488" ht="15.75" customHeight="1"/>
+    <row r="489" ht="15.75" customHeight="1"/>
+    <row r="490" ht="15.75" customHeight="1"/>
+    <row r="491" ht="15.75" customHeight="1"/>
+    <row r="492" ht="15.75" customHeight="1"/>
+    <row r="493" ht="15.75" customHeight="1"/>
+    <row r="494" ht="15.75" customHeight="1"/>
+    <row r="495" ht="15.75" customHeight="1"/>
+    <row r="496" ht="15.75" customHeight="1"/>
+    <row r="497" ht="15.75" customHeight="1"/>
+    <row r="498" ht="15.75" customHeight="1"/>
+    <row r="499" ht="15.75" customHeight="1"/>
+    <row r="500" ht="15.75" customHeight="1"/>
+    <row r="501" ht="15.75" customHeight="1"/>
+    <row r="502" ht="15.75" customHeight="1"/>
+    <row r="503" ht="15.75" customHeight="1"/>
+    <row r="504" ht="15.75" customHeight="1"/>
+    <row r="505" ht="15.75" customHeight="1"/>
+    <row r="506" ht="15.75" customHeight="1"/>
+    <row r="507" ht="15.75" customHeight="1"/>
+    <row r="508" ht="15.75" customHeight="1"/>
+    <row r="509" ht="15.75" customHeight="1"/>
+    <row r="510" ht="15.75" customHeight="1"/>
+    <row r="511" ht="15.75" customHeight="1"/>
+    <row r="512" ht="15.75" customHeight="1"/>
+    <row r="513" ht="15.75" customHeight="1"/>
+    <row r="514" ht="15.75" customHeight="1"/>
+    <row r="515" ht="15.75" customHeight="1"/>
+    <row r="516" ht="15.75" customHeight="1"/>
+    <row r="517" ht="15.75" customHeight="1"/>
+    <row r="518" ht="15.75" customHeight="1"/>
+    <row r="519" ht="15.75" customHeight="1"/>
+    <row r="520" ht="15.75" customHeight="1"/>
+    <row r="521" ht="15.75" customHeight="1"/>
+    <row r="522" ht="15.75" customHeight="1"/>
+    <row r="523" ht="15.75" customHeight="1"/>
+    <row r="524" ht="15.75" customHeight="1"/>
+    <row r="525" ht="15.75" customHeight="1"/>
+    <row r="526" ht="15.75" customHeight="1"/>
+    <row r="527" ht="15.75" customHeight="1"/>
+    <row r="528" ht="15.75" customHeight="1"/>
+    <row r="529" ht="15.75" customHeight="1"/>
+    <row r="530" ht="15.75" customHeight="1"/>
+    <row r="531" ht="15.75" customHeight="1"/>
+    <row r="532" ht="15.75" customHeight="1"/>
+    <row r="533" ht="15.75" customHeight="1"/>
+    <row r="534" ht="15.75" customHeight="1"/>
+    <row r="535" ht="15.75" customHeight="1"/>
+    <row r="536" ht="15.75" customHeight="1"/>
+    <row r="537" ht="15.75" customHeight="1"/>
+    <row r="538" ht="15.75" customHeight="1"/>
+    <row r="539" ht="15.75" customHeight="1"/>
+    <row r="540" ht="15.75" customHeight="1"/>
+    <row r="541" ht="15.75" customHeight="1"/>
+    <row r="542" ht="15.75" customHeight="1"/>
+    <row r="543" ht="15.75" customHeight="1"/>
+    <row r="544" ht="15.75" customHeight="1"/>
+    <row r="545" ht="15.75" customHeight="1"/>
+    <row r="546" ht="15.75" customHeight="1"/>
+    <row r="547" ht="15.75" customHeight="1"/>
+    <row r="548" ht="15.75" customHeight="1"/>
+    <row r="549" ht="15.75" customHeight="1"/>
+    <row r="550" ht="15.75" customHeight="1"/>
+    <row r="551" ht="15.75" customHeight="1"/>
+    <row r="552" ht="15.75" customHeight="1"/>
+    <row r="553" ht="15.75" customHeight="1"/>
+    <row r="554" ht="15.75" customHeight="1"/>
+    <row r="555" ht="15.75" customHeight="1"/>
+    <row r="556" ht="15.75" customHeight="1"/>
+    <row r="557" ht="15.75" customHeight="1"/>
+    <row r="558" ht="15.75" customHeight="1"/>
+    <row r="559" ht="15.75" customHeight="1"/>
+    <row r="560" ht="15.75" customHeight="1"/>
+    <row r="561" ht="15.75" customHeight="1"/>
+    <row r="562" ht="15.75" customHeight="1"/>
+    <row r="563" ht="15.75" customHeight="1"/>
+    <row r="564" ht="15.75" customHeight="1"/>
+    <row r="565" ht="15.75" customHeight="1"/>
+    <row r="566" ht="15.75" customHeight="1"/>
+    <row r="567" ht="15.75" customHeight="1"/>
+    <row r="568" ht="15.75" customHeight="1"/>
+    <row r="569" ht="15.75" customHeight="1"/>
+    <row r="570" ht="15.75" customHeight="1"/>
+    <row r="571" ht="15.75" customHeight="1"/>
+    <row r="572" ht="15.75" customHeight="1"/>
+    <row r="573" ht="15.75" customHeight="1"/>
+    <row r="574" ht="15.75" customHeight="1"/>
+    <row r="575" ht="15.75" customHeight="1"/>
+    <row r="576" ht="15.75" customHeight="1"/>
+    <row r="577" ht="15.75" customHeight="1"/>
+    <row r="578" ht="15.75" customHeight="1"/>
+    <row r="579" ht="15.75" customHeight="1"/>
+    <row r="580" ht="15.75" customHeight="1"/>
+    <row r="581" ht="15.75" customHeight="1"/>
+    <row r="582" ht="15.75" customHeight="1"/>
+    <row r="583" ht="15.75" customHeight="1"/>
+    <row r="584" ht="15.75" customHeight="1"/>
+    <row r="585" ht="15.75" customHeight="1"/>
+    <row r="586" ht="15.75" customHeight="1"/>
+    <row r="587" ht="15.75" customHeight="1"/>
+    <row r="588" ht="15.75" customHeight="1"/>
+    <row r="589" ht="15.75" customHeight="1"/>
+    <row r="590" ht="15.75" customHeight="1"/>
+    <row r="591" ht="15.75" customHeight="1"/>
+    <row r="592" ht="15.75" customHeight="1"/>
+    <row r="593" ht="15.75" customHeight="1"/>
+    <row r="594" ht="15.75" customHeight="1"/>
+    <row r="595" ht="15.75" customHeight="1"/>
+    <row r="596" ht="15.75" customHeight="1"/>
+    <row r="597" ht="15.75" customHeight="1"/>
+    <row r="598" ht="15.75" customHeight="1"/>
+    <row r="599" ht="15.75" customHeight="1"/>
+    <row r="600" ht="15.75" customHeight="1"/>
+    <row r="601" ht="15.75" customHeight="1"/>
+    <row r="602" ht="15.75" customHeight="1"/>
+    <row r="603" ht="15.75" customHeight="1"/>
+    <row r="604" ht="15.75" customHeight="1"/>
+    <row r="605" ht="15.75" customHeight="1"/>
+    <row r="606" ht="15.75" customHeight="1"/>
+    <row r="607" ht="15.75" customHeight="1"/>
+    <row r="608" ht="15.75" customHeight="1"/>
+    <row r="609" ht="15.75" customHeight="1"/>
+    <row r="610" ht="15.75" customHeight="1"/>
+    <row r="611" ht="15.75" customHeight="1"/>
+    <row r="612" ht="15.75" customHeight="1"/>
+    <row r="613" ht="15.75" customHeight="1"/>
+    <row r="614" ht="15.75" customHeight="1"/>
+    <row r="615" ht="15.75" customHeight="1"/>
+    <row r="616" ht="15.75" customHeight="1"/>
+    <row r="617" ht="15.75" customHeight="1"/>
+    <row r="618" ht="15.75" customHeight="1"/>
+    <row r="619" ht="15.75" customHeight="1"/>
+    <row r="620" ht="15.75" customHeight="1"/>
+    <row r="621" ht="15.75" customHeight="1"/>
+    <row r="622" ht="15.75" customHeight="1"/>
+    <row r="623" ht="15.75" customHeight="1"/>
+    <row r="624" ht="15.75" customHeight="1"/>
+    <row r="625" ht="15.75" customHeight="1"/>
+    <row r="626" ht="15.75" customHeight="1"/>
+    <row r="627" ht="15.75" customHeight="1"/>
+    <row r="628" ht="15.75" customHeight="1"/>
+    <row r="629" ht="15.75" customHeight="1"/>
+    <row r="630" ht="15.75" customHeight="1"/>
+    <row r="631" ht="15.75" customHeight="1"/>
+    <row r="632" ht="15.75" customHeight="1"/>
+    <row r="633" ht="15.75" customHeight="1"/>
+    <row r="634" ht="15.75" customHeight="1"/>
+    <row r="635" ht="15.75" customHeight="1"/>
+    <row r="636" ht="15.75" customHeight="1"/>
+    <row r="637" ht="15.75" customHeight="1"/>
+    <row r="638" ht="15.75" customHeight="1"/>
+    <row r="639" ht="15.75" customHeight="1"/>
+    <row r="640" ht="15.75" customHeight="1"/>
+    <row r="641" ht="15.75" customHeight="1"/>
+    <row r="642" ht="15.75" customHeight="1"/>
+    <row r="643" ht="15.75" customHeight="1"/>
+    <row r="644" ht="15.75" customHeight="1"/>
+    <row r="645" ht="15.75" customHeight="1"/>
+    <row r="646" ht="15.75" customHeight="1"/>
+    <row r="647" ht="15.75" customHeight="1"/>
+    <row r="648" ht="15.75" customHeight="1"/>
+    <row r="649" ht="15.75" customHeight="1"/>
+    <row r="650" ht="15.75" customHeight="1"/>
+    <row r="651" ht="15.75" customHeight="1"/>
+    <row r="652" ht="15.75" customHeight="1"/>
+    <row r="653" ht="15.75" customHeight="1"/>
+    <row r="654" ht="15.75" customHeight="1"/>
+    <row r="655" ht="15.75" customHeight="1"/>
+    <row r="656" ht="15.75" customHeight="1"/>
+    <row r="657" ht="15.75" customHeight="1"/>
+    <row r="658" ht="15.75" customHeight="1"/>
+    <row r="659" ht="15.75" customHeight="1"/>
+    <row r="660" ht="15.75" customHeight="1"/>
+    <row r="661" ht="15.75" customHeight="1"/>
+    <row r="662" ht="15.75" customHeight="1"/>
+    <row r="663" ht="15.75" customHeight="1"/>
+    <row r="664" ht="15.75" customHeight="1"/>
+    <row r="665" ht="15.75" customHeight="1"/>
+    <row r="666" ht="15.75" customHeight="1"/>
+    <row r="667" ht="15.75" customHeight="1"/>
+    <row r="668" ht="15.75" customHeight="1"/>
+    <row r="669" ht="15.75" customHeight="1"/>
+    <row r="670" ht="15.75" customHeight="1"/>
+    <row r="671" ht="15.75" customHeight="1"/>
+    <row r="672" ht="15.75" customHeight="1"/>
+    <row r="673" ht="15.75" customHeight="1"/>
+    <row r="674" ht="15.75" customHeight="1"/>
+    <row r="675" ht="15.75" customHeight="1"/>
+    <row r="676" ht="15.75" customHeight="1"/>
+    <row r="677" ht="15.75" customHeight="1"/>
+    <row r="678" ht="15.75" customHeight="1"/>
+    <row r="679" ht="15.75" customHeight="1"/>
+    <row r="680" ht="15.75" customHeight="1"/>
+    <row r="681" ht="15.75" customHeight="1"/>
+    <row r="682" ht="15.75" customHeight="1"/>
+    <row r="683" ht="15.75" customHeight="1"/>
+    <row r="684" ht="15.75" customHeight="1"/>
+    <row r="685" ht="15.75" customHeight="1"/>
+    <row r="686" ht="15.75" customHeight="1"/>
+    <row r="687" ht="15.75" customHeight="1"/>
+    <row r="688" ht="15.75" customHeight="1"/>
+    <row r="689" ht="15.75" customHeight="1"/>
+    <row r="690" ht="15.75" customHeight="1"/>
+    <row r="691" ht="15.75" customHeight="1"/>
+    <row r="692" ht="15.75" customHeight="1"/>
+    <row r="693" ht="15.75" customHeight="1"/>
+    <row r="694" ht="15.75" customHeight="1"/>
+    <row r="695" ht="15.75" customHeight="1"/>
+    <row r="696" ht="15.75" customHeight="1"/>
+    <row r="697" ht="15.75" customHeight="1"/>
+    <row r="698" ht="15.75" customHeight="1"/>
+    <row r="699" ht="15.75" customHeight="1"/>
+    <row r="700" ht="15.75" customHeight="1"/>
+    <row r="701" ht="15.75" customHeight="1"/>
+    <row r="702" ht="15.75" customHeight="1"/>
+    <row r="703" ht="15.75" customHeight="1"/>
+    <row r="704" ht="15.75" customHeight="1"/>
+    <row r="705" ht="15.75" customHeight="1"/>
+    <row r="706" ht="15.75" customHeight="1"/>
+    <row r="707" ht="15.75" customHeight="1"/>
+    <row r="708" ht="15.75" customHeight="1"/>
+    <row r="709" ht="15.75" customHeight="1"/>
+    <row r="710" ht="15.75" customHeight="1"/>
+    <row r="711" ht="15.75" customHeight="1"/>
+    <row r="712" ht="15.75" customHeight="1"/>
+    <row r="713" ht="15.75" customHeight="1"/>
+    <row r="714" ht="15.75" customHeight="1"/>
+    <row r="715" ht="15.75" customHeight="1"/>
+    <row r="716" ht="15.75" customHeight="1"/>
+    <row r="717" ht="15.75" customHeight="1"/>
+    <row r="718" ht="15.75" customHeight="1"/>
+    <row r="719" ht="15.75" customHeight="1"/>
+    <row r="720" ht="15.75" customHeight="1"/>
+    <row r="721" ht="15.75" customHeight="1"/>
+    <row r="722" ht="15.75" customHeight="1"/>
+    <row r="723" ht="15.75" customHeight="1"/>
+    <row r="724" ht="15.75" customHeight="1"/>
+    <row r="725" ht="15.75" customHeight="1"/>
+    <row r="726" ht="15.75" customHeight="1"/>
+    <row r="727" ht="15.75" customHeight="1"/>
+    <row r="728" ht="15.75" customHeight="1"/>
+    <row r="729" ht="15.75" customHeight="1"/>
+    <row r="730" ht="15.75" customHeight="1"/>
+    <row r="731" ht="15.75" customHeight="1"/>
+    <row r="732" ht="15.75" customHeight="1"/>
+    <row r="733" ht="15.75" customHeight="1"/>
+    <row r="734" ht="15.75" customHeight="1"/>
+    <row r="735" ht="15.75" customHeight="1"/>
+    <row r="736" ht="15.75" customHeight="1"/>
+    <row r="737" ht="15.75" customHeight="1"/>
+    <row r="738" ht="15.75" customHeight="1"/>
+    <row r="739" ht="15.75" customHeight="1"/>
+    <row r="740" ht="15.75" customHeight="1"/>
+    <row r="741" ht="15.75" customHeight="1"/>
+    <row r="742" ht="15.75" customHeight="1"/>
+    <row r="743" ht="15.75" customHeight="1"/>
+    <row r="744" ht="15.75" customHeight="1"/>
+    <row r="745" ht="15.75" customHeight="1"/>
+    <row r="746" ht="15.75" customHeight="1"/>
+    <row r="747" ht="15.75" customHeight="1"/>
+    <row r="748" ht="15.75" customHeight="1"/>
+    <row r="749" ht="15.75" customHeight="1"/>
+    <row r="750" ht="15.75" customHeight="1"/>
+    <row r="751" ht="15.75" customHeight="1"/>
+    <row r="752" ht="15.75" customHeight="1"/>
+    <row r="753" ht="15.75" customHeight="1"/>
+    <row r="754" ht="15.75" customHeight="1"/>
+    <row r="755" ht="15.75" customHeight="1"/>
+    <row r="756" ht="15.75" customHeight="1"/>
+    <row r="757" ht="15.75" customHeight="1"/>
+    <row r="758" ht="15.75" customHeight="1"/>
+    <row r="759" ht="15.75" customHeight="1"/>
+    <row r="760" ht="15.75" customHeight="1"/>
+    <row r="761" ht="15.75" customHeight="1"/>
+    <row r="762" ht="15.75" customHeight="1"/>
+    <row r="763" ht="15.75" customHeight="1"/>
+    <row r="764" ht="15.75" customHeight="1"/>
+    <row r="765" ht="15.75" customHeight="1"/>
+    <row r="766" ht="15.75" customHeight="1"/>
+    <row r="767" ht="15.75" customHeight="1"/>
+    <row r="768" ht="15.75" customHeight="1"/>
+    <row r="769" ht="15.75" customHeight="1"/>
+    <row r="770" ht="15.75" customHeight="1"/>
+    <row r="771" ht="15.75" customHeight="1"/>
+    <row r="772" ht="15.75" customHeight="1"/>
+    <row r="773" ht="15.75" customHeight="1"/>
+    <row r="774" ht="15.75" customHeight="1"/>
+    <row r="775" ht="15.75" customHeight="1"/>
+    <row r="776" ht="15.75" customHeight="1"/>
+    <row r="777" ht="15.75" customHeight="1"/>
+    <row r="778" ht="15.75" customHeight="1"/>
+    <row r="779" ht="15.75" customHeight="1"/>
+    <row r="780" ht="15.75" customHeight="1"/>
+    <row r="781" ht="15.75" customHeight="1"/>
+    <row r="782" ht="15.75" customHeight="1"/>
+    <row r="783" ht="15.75" customHeight="1"/>
+    <row r="784" ht="15.75" customHeight="1"/>
+    <row r="785" ht="15.75" customHeight="1"/>
+    <row r="786" ht="15.75" customHeight="1"/>
+    <row r="787" ht="15.75" customHeight="1"/>
+    <row r="788" ht="15.75" customHeight="1"/>
+    <row r="789" ht="15.75" customHeight="1"/>
+    <row r="790" ht="15.75" customHeight="1"/>
+    <row r="791" ht="15.75" customHeight="1"/>
+    <row r="792" ht="15.75" customHeight="1"/>
+    <row r="793" ht="15.75" customHeight="1"/>
+    <row r="794" ht="15.75" customHeight="1"/>
+    <row r="795" ht="15.75" customHeight="1"/>
+    <row r="796" ht="15.75" customHeight="1"/>
+    <row r="797" ht="15.75" customHeight="1"/>
+    <row r="798" ht="15.75" customHeight="1"/>
+    <row r="799" ht="15.75" customHeight="1"/>
+    <row r="800" ht="15.75" customHeight="1"/>
+    <row r="801" ht="15.75" customHeight="1"/>
+    <row r="802" ht="15.75" customHeight="1"/>
+    <row r="803" ht="15.75" customHeight="1"/>
+    <row r="804" ht="15.75" customHeight="1"/>
+    <row r="805" ht="15.75" customHeight="1"/>
+    <row r="806" ht="15.75" customHeight="1"/>
+    <row r="807" ht="15.75" customHeight="1"/>
+    <row r="808" ht="15.75" customHeight="1"/>
+    <row r="809" ht="15.75" customHeight="1"/>
+    <row r="810" ht="15.75" customHeight="1"/>
+    <row r="811" ht="15.75" customHeight="1"/>
+    <row r="812" ht="15.75" customHeight="1"/>
+    <row r="813" ht="15.75" customHeight="1"/>
+    <row r="814" ht="15.75" customHeight="1"/>
+    <row r="815" ht="15.75" customHeight="1"/>
+    <row r="816" ht="15.75" customHeight="1"/>
+    <row r="817" ht="15.75" customHeight="1"/>
+    <row r="818" ht="15.75" customHeight="1"/>
+    <row r="819" ht="15.75" customHeight="1"/>
+    <row r="820" ht="15.75" customHeight="1"/>
+    <row r="821" ht="15.75" customHeight="1"/>
+    <row r="822" ht="15.75" customHeight="1"/>
+    <row r="823" ht="15.75" customHeight="1"/>
+    <row r="824" ht="15.75" customHeight="1"/>
+    <row r="825" ht="15.75" customHeight="1"/>
+    <row r="826" ht="15.75" customHeight="1"/>
+    <row r="827" ht="15.75" customHeight="1"/>
+    <row r="828" ht="15.75" customHeight="1"/>
+    <row r="829" ht="15.75" customHeight="1"/>
+    <row r="830" ht="15.75" customHeight="1"/>
+    <row r="831" ht="15.75" customHeight="1"/>
+    <row r="832" ht="15.75" customHeight="1"/>
+    <row r="833" ht="15.75" customHeight="1"/>
+    <row r="834" ht="15.75" customHeight="1"/>
+    <row r="835" ht="15.75" customHeight="1"/>
+    <row r="836" ht="15.75" customHeight="1"/>
+    <row r="837" ht="15.75" customHeight="1"/>
+    <row r="838" ht="15.75" customHeight="1"/>
+    <row r="839" ht="15.75" customHeight="1"/>
+    <row r="840" ht="15.75" customHeight="1"/>
+    <row r="841" ht="15.75" customHeight="1"/>
+    <row r="842" ht="15.75" customHeight="1"/>
+    <row r="843" ht="15.75" customHeight="1"/>
+    <row r="844" ht="15.75" customHeight="1"/>
+    <row r="845" ht="15.75" customHeight="1"/>
+    <row r="846" ht="15.75" customHeight="1"/>
+    <row r="847" ht="15.75" customHeight="1"/>
+    <row r="848" ht="15.75" customHeight="1"/>
+    <row r="849" ht="15.75" customHeight="1"/>
+    <row r="850" ht="15.75" customHeight="1"/>
+    <row r="851" ht="15.75" customHeight="1"/>
+    <row r="852" ht="15.75" customHeight="1"/>
+    <row r="853" ht="15.75" customHeight="1"/>
+    <row r="854" ht="15.75" customHeight="1"/>
+    <row r="855" ht="15.75" customHeight="1"/>
+    <row r="856" ht="15.75" customHeight="1"/>
+    <row r="857" ht="15.75" customHeight="1"/>
+    <row r="858" ht="15.75" customHeight="1"/>
+    <row r="859" ht="15.75" customHeight="1"/>
+    <row r="860" ht="15.75" customHeight="1"/>
+    <row r="861" ht="15.75" customHeight="1"/>
+    <row r="862" ht="15.75" customHeight="1"/>
+    <row r="863" ht="15.75" customHeight="1"/>
+    <row r="864" ht="15.75" customHeight="1"/>
+    <row r="865" ht="15.75" customHeight="1"/>
+    <row r="866" ht="15.75" customHeight="1"/>
+    <row r="867" ht="15.75" customHeight="1"/>
+    <row r="868" ht="15.75" customHeight="1"/>
+    <row r="869" ht="15.75" customHeight="1"/>
+    <row r="870" ht="15.75" customHeight="1"/>
+    <row r="871" ht="15.75" customHeight="1"/>
+    <row r="872" ht="15.75" customHeight="1"/>
+    <row r="873" ht="15.75" customHeight="1"/>
+    <row r="874" ht="15.75" customHeight="1"/>
+    <row r="875" ht="15.75" customHeight="1"/>
+    <row r="876" ht="15.75" customHeight="1"/>
+    <row r="877" ht="15.75" customHeight="1"/>
+    <row r="878" ht="15.75" customHeight="1"/>
+    <row r="879" ht="15.75" customHeight="1"/>
+    <row r="880" ht="15.75" customHeight="1"/>
+    <row r="881" ht="15.75" customHeight="1"/>
+    <row r="882" ht="15.75" customHeight="1"/>
+    <row r="883" ht="15.75" customHeight="1"/>
+    <row r="884" ht="15.75" customHeight="1"/>
+    <row r="885" ht="15.75" customHeight="1"/>
+    <row r="886" ht="15.75" customHeight="1"/>
+    <row r="887" ht="15.75" customHeight="1"/>
+    <row r="888" ht="15.75" customHeight="1"/>
+    <row r="889" ht="15.75" customHeight="1"/>
+    <row r="890" ht="15.75" customHeight="1"/>
+    <row r="891" ht="15.75" customHeight="1"/>
+    <row r="892" ht="15.75" customHeight="1"/>
+    <row r="893" ht="15.75" customHeight="1"/>
+    <row r="894" ht="15.75" customHeight="1"/>
+    <row r="895" ht="15.75" customHeight="1"/>
+    <row r="896" ht="15.75" customHeight="1"/>
+    <row r="897" ht="15.75" customHeight="1"/>
+    <row r="898" ht="15.75" customHeight="1"/>
+    <row r="899" ht="15.75" customHeight="1"/>
+    <row r="900" ht="15.75" customHeight="1"/>
+    <row r="901" ht="15.75" customHeight="1"/>
+    <row r="902" ht="15.75" customHeight="1"/>
+    <row r="903" ht="15.75" customHeight="1"/>
+    <row r="904" ht="15.75" customHeight="1"/>
+    <row r="905" ht="15.75" customHeight="1"/>
+    <row r="906" ht="15.75" customHeight="1"/>
+    <row r="907" ht="15.75" customHeight="1"/>
+    <row r="908" ht="15.75" customHeight="1"/>
+    <row r="909" ht="15.75" customHeight="1"/>
+    <row r="910" ht="15.75" customHeight="1"/>
+    <row r="911" ht="15.75" customHeight="1"/>
+    <row r="912" ht="15.75" customHeight="1"/>
+    <row r="913" ht="15.75" customHeight="1"/>
+    <row r="914" ht="15.75" customHeight="1"/>
+    <row r="915" ht="15.75" customHeight="1"/>
+    <row r="916" ht="15.75" customHeight="1"/>
+    <row r="917" ht="15.75" customHeight="1"/>
+    <row r="918" ht="15.75" customHeight="1"/>
+    <row r="919" ht="15.75" customHeight="1"/>
+    <row r="920" ht="15.75" customHeight="1"/>
+    <row r="921" ht="15.75" customHeight="1"/>
+    <row r="922" ht="15.75" customHeight="1"/>
+    <row r="923" ht="15.75" customHeight="1"/>
+    <row r="924" ht="15.75" customHeight="1"/>
+    <row r="925" ht="15.75" customHeight="1"/>
+    <row r="926" ht="15.75" customHeight="1"/>
+    <row r="927" ht="15.75" customHeight="1"/>
+    <row r="928" ht="15.75" customHeight="1"/>
+    <row r="929" ht="15.75" customHeight="1"/>
+    <row r="930" ht="15.75" customHeight="1"/>
+    <row r="931" ht="15.75" customHeight="1"/>
+    <row r="932" ht="15.75" customHeight="1"/>
+    <row r="933" ht="15.75" customHeight="1"/>
+    <row r="934" ht="15.75" customHeight="1"/>
+    <row r="935" ht="15.75" customHeight="1"/>
+    <row r="936" ht="15.75" customHeight="1"/>
+    <row r="937" ht="15.75" customHeight="1"/>
+    <row r="938" ht="15.75" customHeight="1"/>
+    <row r="939" ht="15.75" customHeight="1"/>
+    <row r="940" ht="15.75" customHeight="1"/>
+    <row r="941" ht="15.75" customHeight="1"/>
+    <row r="942" ht="15.75" customHeight="1"/>
+    <row r="943" ht="15.75" customHeight="1"/>
+    <row r="944" ht="15.75" customHeight="1"/>
+    <row r="945" ht="15.75" customHeight="1"/>
+    <row r="946" ht="15.75" customHeight="1"/>
+    <row r="947" ht="15.75" customHeight="1"/>
+    <row r="948" ht="15.75" customHeight="1"/>
+    <row r="949" ht="15.75" customHeight="1"/>
+    <row r="950" ht="15.75" customHeight="1"/>
+    <row r="951" ht="15.75" customHeight="1"/>
+    <row r="952" ht="15.75" customHeight="1"/>
+    <row r="953" ht="15.75" customHeight="1"/>
+    <row r="954" ht="15.75" customHeight="1"/>
+    <row r="955" ht="15.75" customHeight="1"/>
+    <row r="956" ht="15.75" customHeight="1"/>
+    <row r="957" ht="15.75" customHeight="1"/>
+    <row r="958" ht="15.75" customHeight="1"/>
+    <row r="959" ht="15.75" customHeight="1"/>
+    <row r="960" ht="15.75" customHeight="1"/>
+    <row r="961" ht="15.75" customHeight="1"/>
+    <row r="962" ht="15.75" customHeight="1"/>
+    <row r="963" ht="15.75" customHeight="1"/>
+    <row r="964" ht="15.75" customHeight="1"/>
+    <row r="965" ht="15.75" customHeight="1"/>
+    <row r="966" ht="15.75" customHeight="1"/>
+    <row r="967" ht="15.75" customHeight="1"/>
+    <row r="968" ht="15.75" customHeight="1"/>
+    <row r="969" ht="15.75" customHeight="1"/>
+    <row r="970" ht="15.75" customHeight="1"/>
+    <row r="971" ht="15.75" customHeight="1"/>
+    <row r="972" ht="15.75" customHeight="1"/>
+    <row r="973" ht="15.75" customHeight="1"/>
+    <row r="974" ht="15.75" customHeight="1"/>
+    <row r="975" ht="15.75" customHeight="1"/>
+    <row r="976" ht="15.75" customHeight="1"/>
+    <row r="977" ht="15.75" customHeight="1"/>
+    <row r="978" ht="15.75" customHeight="1"/>
+    <row r="979" ht="15.75" customHeight="1"/>
+    <row r="980" ht="15.75" customHeight="1"/>
+    <row r="981" ht="15.75" customHeight="1"/>
+    <row r="982" ht="15.75" customHeight="1"/>
+    <row r="983" ht="15.75" customHeight="1"/>
+    <row r="984" ht="15.75" customHeight="1"/>
+    <row r="985" ht="15.75" customHeight="1"/>
+    <row r="986" ht="15.75" customHeight="1"/>
+    <row r="987" ht="15.75" customHeight="1"/>
+    <row r="988" ht="15.75" customHeight="1"/>
+    <row r="989" ht="15.75" customHeight="1"/>
+    <row r="990" ht="15.75" customHeight="1"/>
+    <row r="991" ht="15.75" customHeight="1"/>
+    <row r="992" ht="15.75" customHeight="1"/>
+    <row r="993" ht="15.75" customHeight="1"/>
+    <row r="994" ht="15.75" customHeight="1"/>
+    <row r="995" ht="15.75" customHeight="1"/>
+    <row r="996" ht="15.75" customHeight="1"/>
+    <row r="997" ht="15.75" customHeight="1"/>
+    <row r="998" ht="15.75" customHeight="1"/>
+    <row r="999" ht="15.75" customHeight="1"/>
+    <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>